<commit_message>
updated OSHpark PCB price for volume production
PCB price is 5x lower if order is > 150 square inches
</commit_message>
<xml_diff>
--- a/hardware/eagle/bom.xlsx
+++ b/hardware/eagle/bom.xlsx
@@ -2321,7 +2321,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2520,8 +2520,8 @@
         <v>5.9466666666666663</v>
       </c>
       <c r="I5" s="3">
-        <f>17.84/3</f>
-        <v>5.9466666666666663</v>
+        <f>Tableau3[[#This Row],[€ / u / 1pc]]/5</f>
+        <v>1.1893333333333334</v>
       </c>
       <c r="J5" s="3">
         <f>G5*H5</f>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="K5" s="3">
         <f>G5*I5</f>
-        <v>5.9466666666666663</v>
+        <v>1.1893333333333334</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>115</v>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="K22" s="8">
         <f>SUM(K3:K21)</f>
-        <v>28.027666666666669</v>
+        <v>23.270333333333337</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>

</xml_diff>

<commit_message>
added power indicating led
fix #1
added green led to indicate power on the 5V rail.
</commit_message>
<xml_diff>
--- a/hardware/eagle/bom.xlsx
+++ b/hardware/eagle/bom.xlsx
@@ -11,19 +11,15 @@
     <sheet name="other" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$2:$M$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$2:$M$23</definedName>
     <definedName name="PlageNommée1">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
-  <si>
-    <t>AirCat audio shield - BOM - ver. hw_0.0.3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="156">
   <si>
     <t>category</t>
   </si>
@@ -461,6 +457,36 @@
   </si>
   <si>
     <t>http://www.ebay.com/itm/2pcs-Video-AV-Balun-3-5mm-1-8-stereo-male-plug-to-AV-Screw-Terminal-Plug-adapter-/231204744595?pt=LH_DefaultDomain_0&amp;hash=item35d4e06d93</t>
+  </si>
+  <si>
+    <t>SMD 0603" 150R</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/multicomp/mcmr06x1500ftl/resistance-0603-150r-1-anti-sulfur/dp/2073388</t>
+  </si>
+  <si>
+    <t>MCMR06X1500FTL</t>
+  </si>
+  <si>
+    <t>led</t>
+  </si>
+  <si>
+    <t>SMD 0603" Green 10mcd</t>
+  </si>
+  <si>
+    <t>KINGBRIGHT</t>
+  </si>
+  <si>
+    <t>KP-1608SGC</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/kingbright/kp-1608sgc/led-cms-0603-vert/dp/8529833</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/55768.pdf</t>
+  </si>
+  <si>
+    <t>AirCat audio shield - BOM</t>
   </si>
 </sst>
 </file>
@@ -471,14 +497,9 @@
     <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -560,6 +581,25 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -873,453 +913,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="16" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1347,106 +1004,12 @@
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
+        <right/>
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6FA8DC"/>
-          <bgColor rgb="FF6FA8DC"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1509,6 +1072,42 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1524,6 +1123,42 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1583,7 +1218,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1591,7 +1225,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1601,11 +1235,7 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1665,6 +1295,42 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
       <fill>
         <patternFill patternType="none">
@@ -1713,6 +1379,43 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1753,6 +1456,42 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1793,6 +1532,42 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1833,6 +1608,42 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1873,6 +1684,42 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1913,6 +1760,42 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1953,6 +1836,116 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1977,25 +1970,83 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6FA8DC"/>
+          <bgColor rgb="FF6FA8DC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -2004,29 +2055,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A2:M21" headerRowDxfId="13" dataDxfId="14" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
-  <autoFilter ref="A2:M21"/>
-  <sortState ref="A3:M21">
-    <sortCondition descending="1" ref="J2:J21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A2:M23" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A2:M23"/>
+  <sortState ref="A3:M23">
+    <sortCondition descending="1" ref="K2:K23"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="category" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="0"/>
-    <tableColumn id="2" name="value/description" dataDxfId="26" totalsRowDxfId="1"/>
-    <tableColumn id="3" name="manufacturer name" dataDxfId="25" totalsRowDxfId="2"/>
-    <tableColumn id="4" name="manufacturer ref" dataDxfId="24" totalsRowDxfId="3"/>
-    <tableColumn id="5" name="vendor name" dataDxfId="23" totalsRowDxfId="4"/>
-    <tableColumn id="6" name="vendor ref" dataDxfId="22" totalsRowDxfId="5"/>
-    <tableColumn id="7" name="qty" dataDxfId="21" totalsRowDxfId="6"/>
-    <tableColumn id="8" name="€ / u / 1pc" dataDxfId="20" totalsRowDxfId="7"/>
-    <tableColumn id="9" name="€ / u / 100pcs" dataDxfId="19" totalsRowDxfId="8"/>
-    <tableColumn id="10" name="€ / 1pc" dataDxfId="18" totalsRowDxfId="9">
+    <tableColumn id="1" name="category" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="value/description" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="manufacturer name" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="manufacturer ref" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="vendor name" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="vendor ref" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="7" name="qty" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="8" name="€ / u / 1pc" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="9" name="€ / u / 100pcs" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="10" name="€ / 1pc" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>G3*H3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="€ / 100pc" dataDxfId="17" totalsRowDxfId="10">
+    <tableColumn id="11" name="€ / 100pc" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>G3*I3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="link" dataDxfId="16" totalsRowDxfId="11"/>
-    <tableColumn id="13" name="datasheet" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="12"/>
+    <tableColumn id="12" name="link" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="13" name="datasheet" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2317,11 +2368,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE73"/>
+  <dimension ref="A1:AE75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2342,59 +2393,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+    </row>
+    <row r="2" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>12</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>13</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -2416,20 +2467,20 @@
       <c r="AE2" s="1"/>
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="F3" s="2">
         <v>1882283</v>
@@ -2451,28 +2502,28 @@
         <f>G3*I3</f>
         <v>10.41</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="15" t="s">
+    </row>
+    <row r="4" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A4" s="13" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A4" s="14" t="s">
+      <c r="B4" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="F4" s="2">
         <v>1689419</v>
@@ -2494,149 +2545,149 @@
         <f>G4*I4</f>
         <v>5.83</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="M4" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="M4" s="15" t="s">
+    </row>
+    <row r="5" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A5" s="13" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A5" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="2">
+        <v>9306803</v>
+      </c>
       <c r="G5" s="2">
         <v>1</v>
       </c>
       <c r="H5" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.51</v>
+      </c>
+      <c r="J5" s="3">
+        <f>G5*H5</f>
+        <v>1.7</v>
+      </c>
+      <c r="K5" s="3">
+        <f>G5*I5</f>
+        <v>1.51</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A6" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
         <f>17.84/3</f>
         <v>5.9466666666666663</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I6" s="3">
         <f>Tableau3[[#This Row],[€ / u / 1pc]]/5</f>
         <v>1.1893333333333334</v>
       </c>
-      <c r="J5" s="3">
-        <f>G5*H5</f>
-        <v>5.9466666666666663</v>
-      </c>
-      <c r="K5" s="3">
-        <f>G5*I5</f>
-        <v>1.1893333333333334</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="M5" s="16"/>
-    </row>
-    <row r="6" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2">
-        <v>2254444</v>
-      </c>
-      <c r="G6" s="2">
-        <v>7</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.41</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.14799999999999999</v>
-      </c>
       <c r="J6" s="3">
         <f>G6*H6</f>
-        <v>2.8699999999999997</v>
+        <v>5.9466666666666663</v>
       </c>
       <c r="K6" s="3">
         <f>G6*I6</f>
-        <v>1.036</v>
+        <v>1.1893333333333334</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>20</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A7" s="14" t="s">
-        <v>106</v>
+      <c r="A7" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>109</v>
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2">
-        <v>9306803</v>
+        <v>2254444</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H7" s="3">
-        <v>1.7</v>
+        <v>0.41</v>
       </c>
       <c r="I7" s="3">
-        <v>1.51</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="J7" s="3">
         <f>G7*H7</f>
-        <v>1.7</v>
+        <v>2.8699999999999997</v>
       </c>
       <c r="K7" s="3">
         <f>G7*I7</f>
-        <v>1.51</v>
-      </c>
-      <c r="L7" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="M7" s="15" t="s">
-        <v>112</v>
+        <v>1.036</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="F8" s="2">
         <v>1759136</v>
@@ -2659,27 +2710,27 @@
         <v>1.008</v>
       </c>
       <c r="L8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="M8" s="15" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="F9" s="2">
         <v>1593445</v>
@@ -2701,31 +2752,31 @@
         <f>G9*I9</f>
         <v>0.64</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="M9" s="15" t="s">
+    </row>
+    <row r="10" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A10" s="13" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A10" s="14" t="s">
+      <c r="B10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="F10" s="24" t="s">
         <v>82</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>83</v>
       </c>
       <c r="G10" s="2">
         <v>2</v>
@@ -2744,26 +2795,26 @@
         <f>G10*I10</f>
         <v>0.64</v>
       </c>
-      <c r="L10" s="27" t="s">
+      <c r="L10" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A11" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="M10" s="16"/>
-    </row>
-    <row r="11" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A11" s="14" t="s">
+      <c r="B11" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="F11" s="2">
         <v>1593440</v>
@@ -2786,29 +2837,29 @@
         <v>0.32</v>
       </c>
       <c r="L11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="15" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="E12" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="F12" s="24">
+      <c r="F12" s="23">
         <v>2073537</v>
       </c>
       <c r="G12" s="2">
@@ -2828,28 +2879,28 @@
         <f>G12*I12</f>
         <v>0.128</v>
       </c>
-      <c r="L12" s="26" t="s">
+      <c r="L12" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="M12" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="M12" s="15" t="s">
+    </row>
+    <row r="13" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A13" s="13" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A13" s="14" t="s">
+      <c r="B13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="F13" s="2">
         <v>2073570</v>
@@ -2871,114 +2922,114 @@
         <f>G13*I13</f>
         <v>0.128</v>
       </c>
-      <c r="L13" s="26" t="s">
+      <c r="L13" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="M13" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="M13" s="15" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A14" s="14" t="s">
-        <v>21</v>
+      <c r="A14" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1759083</v>
+        <v>31</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="G14" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H14" s="3">
-        <v>7.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="I14" s="3">
-        <v>6.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="J14" s="3">
         <f>G14*H14</f>
-        <v>0.112</v>
+        <v>0.10799999999999998</v>
       </c>
       <c r="K14" s="3">
         <f>G14*I14</f>
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="L14" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>27</v>
+        <v>0.10799999999999998</v>
+      </c>
+      <c r="L14" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A15" s="14" t="s">
-        <v>28</v>
+      <c r="A15" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1759083</v>
       </c>
       <c r="G15" s="2">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H15" s="3">
-        <v>8.9999999999999993E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="I15" s="3">
-        <v>8.9999999999999993E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="J15" s="3">
         <f>G15*H15</f>
-        <v>0.10799999999999998</v>
+        <v>0.112</v>
       </c>
       <c r="K15" s="3">
         <f>G15*I15</f>
-        <v>0.10799999999999998</v>
-      </c>
-      <c r="L15" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="M15" s="15" t="s">
-        <v>35</v>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="E16" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="F16" s="2">
         <v>1759009</v>
@@ -3000,74 +3051,74 @@
         <f>G16*I16</f>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="L16" s="26" t="s">
+      <c r="L16" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="M16" s="15" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>52</v>
+      <c r="A17" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>151</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>54</v>
+        <v>152</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>17</v>
       </c>
       <c r="F17" s="2">
-        <v>1759027</v>
+        <v>8529833</v>
       </c>
       <c r="G17" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H17" s="3">
-        <v>8.9999999999999993E-3</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="I17" s="3">
-        <v>8.0000000000000002E-3</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="J17" s="3">
         <f>G17*H17</f>
-        <v>5.3999999999999992E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="K17" s="3">
         <f>G17*I17</f>
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="M17" s="15" t="s">
-        <v>56</v>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L17" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="M17" s="41" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="14" t="s">
-        <v>57</v>
+      <c r="A18" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F18" s="2">
-        <v>2320806</v>
+        <v>1759027</v>
       </c>
       <c r="G18" s="2">
         <v>6</v>
@@ -3087,174 +3138,252 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M18" s="15" t="s">
-        <v>63</v>
+        <v>54</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="14" t="s">
-        <v>64</v>
+      <c r="A19" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F19" s="2">
-        <v>1759037</v>
+        <v>2320806</v>
       </c>
       <c r="G19" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H19" s="3">
-        <v>7.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="I19" s="3">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="J19" s="3">
         <f>G19*H19</f>
-        <v>3.5000000000000003E-2</v>
+        <v>5.3999999999999992E-2</v>
       </c>
       <c r="K19" s="3">
         <f>G19*I19</f>
-        <v>0.03</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="M19" s="15" t="s">
-        <v>70</v>
+        <v>61</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="14" t="s">
-        <v>130</v>
+      <c r="A20" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
       <c r="F20" s="2">
-        <v>2073461</v>
+        <v>1759037</v>
       </c>
       <c r="G20" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H20" s="3">
-        <v>8.0000000000000002E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="I20" s="3">
-        <v>8.0000000000000002E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="J20" s="3">
         <f>G20*H20</f>
-        <v>2.4E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="K20" s="3">
         <f>G20*I20</f>
+        <v>0.03</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A21" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2073461</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3</v>
+      </c>
+      <c r="H21" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I21" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J21" s="3">
+        <f>G21*H21</f>
         <v>2.4E-2</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="K21" s="3">
+        <f>G21*I21</f>
+        <v>2.4E-2</v>
+      </c>
+      <c r="L21" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="M21" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="M20" s="15" t="s">
+    </row>
+    <row r="22" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A22" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2073388</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I22" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="J22" s="3">
+        <f>G22*H22</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="K22" s="3">
+        <f>G22*I22</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="L22" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="M22" s="39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A23" s="27" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="28" t="s">
+      <c r="B23" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="D23" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="E23" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="F23" s="28">
+        <v>9238760</v>
+      </c>
+      <c r="G23" s="28">
+        <v>1</v>
+      </c>
+      <c r="H23" s="29">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I23" s="29">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J23" s="30">
+        <f>G23*H23</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K23" s="30">
+        <f>G23*I23</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L23" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="F21" s="29">
-        <v>9238760</v>
-      </c>
-      <c r="G21" s="29">
-        <v>1</v>
-      </c>
-      <c r="H21" s="30">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="I21" s="30">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="J21" s="31">
-        <f>G21*H21</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="K21" s="31">
-        <f>G21*I21</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="L21" s="32" t="s">
+      <c r="M23" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="M21" s="33" t="s">
+    </row>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A24" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7">
-        <f>SUM(G3:G21)</f>
-        <v>127</v>
-      </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="8">
-        <f>SUM(J3:J21)</f>
-        <v>40.654666666666671</v>
-      </c>
-      <c r="K22" s="8">
-        <f>SUM(K3:K21)</f>
-        <v>23.270333333333337</v>
-      </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7">
+        <f>SUM(G3:G23)</f>
+        <v>129</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="8">
+        <f>SUM(J3:J23)</f>
+        <v>40.739666666666672</v>
+      </c>
+      <c r="K24" s="8">
+        <f>SUM(K3:K23)</f>
+        <v>23.348333333333336</v>
+      </c>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="H25" s="9"/>
@@ -3451,28 +3580,36 @@
     <row r="73" spans="8:9" ht="15.75" customHeight="1">
       <c r="H73" s="9"/>
       <c r="I73" s="9"/>
+    </row>
+    <row r="74" spans="8:9" ht="15.75" customHeight="1">
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="8:9" ht="15.75" customHeight="1">
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L6" r:id="rId1"/>
-    <hyperlink ref="M6" r:id="rId2"/>
-    <hyperlink ref="L14" r:id="rId3"/>
-    <hyperlink ref="M14" r:id="rId4"/>
-    <hyperlink ref="L15" r:id="rId5"/>
-    <hyperlink ref="M15" r:id="rId6"/>
+    <hyperlink ref="L7" r:id="rId1"/>
+    <hyperlink ref="M7" r:id="rId2"/>
+    <hyperlink ref="L15" r:id="rId3"/>
+    <hyperlink ref="M15" r:id="rId4"/>
+    <hyperlink ref="L14" r:id="rId5"/>
+    <hyperlink ref="M14" r:id="rId6"/>
     <hyperlink ref="L8" r:id="rId7"/>
     <hyperlink ref="M8" r:id="rId8"/>
     <hyperlink ref="L16" r:id="rId9"/>
     <hyperlink ref="M16" r:id="rId10"/>
-    <hyperlink ref="L17" r:id="rId11"/>
-    <hyperlink ref="M17" r:id="rId12"/>
-    <hyperlink ref="L18" r:id="rId13"/>
-    <hyperlink ref="M18" r:id="rId14"/>
-    <hyperlink ref="L19" r:id="rId15"/>
-    <hyperlink ref="M19" r:id="rId16"/>
+    <hyperlink ref="L18" r:id="rId11"/>
+    <hyperlink ref="M18" r:id="rId12"/>
+    <hyperlink ref="L19" r:id="rId13"/>
+    <hyperlink ref="M19" r:id="rId14"/>
+    <hyperlink ref="L20" r:id="rId15"/>
+    <hyperlink ref="M20" r:id="rId16"/>
     <hyperlink ref="L9" r:id="rId17"/>
     <hyperlink ref="M9" r:id="rId18"/>
     <hyperlink ref="L10" r:id="rId19"/>
@@ -3482,18 +3619,18 @@
     <hyperlink ref="M3" r:id="rId23"/>
     <hyperlink ref="L4" r:id="rId24"/>
     <hyperlink ref="M4" r:id="rId25"/>
-    <hyperlink ref="L7" r:id="rId26"/>
-    <hyperlink ref="M7" r:id="rId27"/>
-    <hyperlink ref="E5" r:id="rId28"/>
-    <hyperlink ref="L5" r:id="rId29"/>
+    <hyperlink ref="L5" r:id="rId26"/>
+    <hyperlink ref="M5" r:id="rId27"/>
+    <hyperlink ref="E6" r:id="rId28"/>
+    <hyperlink ref="L6" r:id="rId29"/>
     <hyperlink ref="L12" r:id="rId30"/>
     <hyperlink ref="M12" r:id="rId31"/>
     <hyperlink ref="L13" r:id="rId32"/>
     <hyperlink ref="M13" r:id="rId33"/>
-    <hyperlink ref="L20" r:id="rId34"/>
-    <hyperlink ref="M20" r:id="rId35"/>
-    <hyperlink ref="L21" r:id="rId36"/>
-    <hyperlink ref="M21" r:id="rId37"/>
+    <hyperlink ref="L21" r:id="rId34"/>
+    <hyperlink ref="M21" r:id="rId35"/>
+    <hyperlink ref="L23" r:id="rId36"/>
+    <hyperlink ref="M23" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
@@ -3517,10 +3654,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>145</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added SPDIF OUT connector
fix #4
</commit_message>
<xml_diff>
--- a/hardware/eagle/bom.xlsx
+++ b/hardware/eagle/bom.xlsx
@@ -11,7 +11,7 @@
     <sheet name="other" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$2:$M$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$2:$M$24</definedName>
     <definedName name="PlageNommée1">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="160">
   <si>
     <t>category</t>
   </si>
@@ -487,6 +487,18 @@
   </si>
   <si>
     <t>AirCat audio shield - BOM</t>
+  </si>
+  <si>
+    <t>0.05" male SMD 1x2</t>
+  </si>
+  <si>
+    <t>2211S-02G</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/multicomp/2211s-02g/embase-male-1-rangee-vert-2voies/dp/1593411</t>
+  </si>
+  <si>
+    <t>http://www.farnell.com/datasheets/1518407.pdf</t>
   </si>
 </sst>
 </file>
@@ -497,7 +509,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -600,6 +612,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -920,13 +939,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="14" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -971,6 +989,9 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2055,8 +2076,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A2:M23" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="A2:M23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A2:M24" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A2:M24"/>
   <sortState ref="A3:M23">
     <sortCondition descending="1" ref="K2:K23"/>
   </sortState>
@@ -2368,11 +2389,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE75"/>
+  <dimension ref="A1:AE76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:K1"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2393,58 +2414,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="17" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="1"/>
@@ -2467,7 +2488,7 @@
       <c r="AE2" s="1"/>
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2495,22 +2516,22 @@
         <v>3.47</v>
       </c>
       <c r="J3" s="3">
-        <f>G3*H3</f>
+        <f t="shared" ref="J3:J24" si="0">G3*H3</f>
         <v>14.64</v>
       </c>
       <c r="K3" s="3">
-        <f>G3*I3</f>
+        <f t="shared" ref="K3:K24" si="1">G3*I3</f>
         <v>10.41</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>98</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2538,22 +2559,22 @@
         <v>5.83</v>
       </c>
       <c r="J4" s="3">
-        <f>G4*H4</f>
+        <f t="shared" si="0"/>
         <v>11.86</v>
       </c>
       <c r="K4" s="3">
-        <f>G4*I4</f>
+        <f t="shared" si="1"/>
         <v>5.83</v>
       </c>
-      <c r="L4" s="26" t="s">
+      <c r="L4" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="13" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>105</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2562,7 +2583,7 @@
       <c r="C5" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>108</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -2581,28 +2602,28 @@
         <v>1.51</v>
       </c>
       <c r="J5" s="3">
-        <f>G5*H5</f>
+        <f t="shared" si="0"/>
         <v>1.7</v>
       </c>
       <c r="K5" s="3">
-        <f>G5*I5</f>
+        <f t="shared" si="1"/>
         <v>1.51</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="L5" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="13" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>113</v>
       </c>
       <c r="F6" s="2"/>
@@ -2618,20 +2639,20 @@
         <v>1.1893333333333334</v>
       </c>
       <c r="J6" s="3">
-        <f>G6*H6</f>
+        <f t="shared" si="0"/>
         <v>5.9466666666666663</v>
       </c>
       <c r="K6" s="3">
-        <f>G6*I6</f>
+        <f t="shared" si="1"/>
         <v>1.1893333333333334</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="M6" s="15"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2659,22 +2680,22 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="J7" s="3">
-        <f>G7*H7</f>
+        <f t="shared" si="0"/>
         <v>2.8699999999999997</v>
       </c>
       <c r="K7" s="3">
-        <f>G7*I7</f>
+        <f t="shared" si="1"/>
         <v>1.036</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2702,22 +2723,22 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="J8" s="3">
-        <f>G8*H8</f>
+        <f t="shared" si="0"/>
         <v>1.008</v>
       </c>
       <c r="K8" s="3">
-        <f>G8*I8</f>
+        <f t="shared" si="1"/>
         <v>1.008</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>70</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2745,37 +2766,37 @@
         <v>0.64</v>
       </c>
       <c r="J9" s="3">
-        <f>G9*H9</f>
+        <f t="shared" si="0"/>
         <v>0.83</v>
       </c>
       <c r="K9" s="3">
-        <f>G9*I9</f>
+        <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
-      <c r="L9" s="26" t="s">
+      <c r="L9" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="M9" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>77</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="23" t="s">
         <v>82</v>
       </c>
       <c r="G10" s="2">
@@ -2788,122 +2809,122 @@
         <v>0.32</v>
       </c>
       <c r="J10" s="3">
-        <f>G10*H10</f>
+        <f t="shared" si="0"/>
         <v>0.72</v>
       </c>
       <c r="K10" s="3">
-        <f>G10*I10</f>
+        <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
-      <c r="L10" s="26" t="s">
+      <c r="L10" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="M10" s="15"/>
-    </row>
-    <row r="11" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A11" s="13" t="s">
-        <v>84</v>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:31" s="36" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A11" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1593440</v>
+        <v>156</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="22">
+        <v>1593411</v>
       </c>
       <c r="G11" s="2">
         <v>1</v>
       </c>
       <c r="H11" s="3">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" ref="J11" si="2">G11*H11</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" ref="K11" si="3">G11*I11</f>
+        <v>2.7E-2</v>
+      </c>
+      <c r="L11" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="M11" s="45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A12" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1593440</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
         <v>0.36</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I12" s="3">
         <v>0.32</v>
       </c>
-      <c r="J11" s="3">
-        <f>G11*H11</f>
+      <c r="J12" s="3">
+        <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="K11" s="3">
-        <f>G11*I11</f>
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L12" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="M12" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A12" s="13" t="s">
+    <row r="13" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A13" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E13" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F13" s="22">
         <v>2073537</v>
-      </c>
-      <c r="G12" s="2">
-        <v>16</v>
-      </c>
-      <c r="H12" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I12" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="J12" s="3">
-        <f>G12*H12</f>
-        <v>0.128</v>
-      </c>
-      <c r="K12" s="3">
-        <f>G12*I12</f>
-        <v>0.128</v>
-      </c>
-      <c r="L12" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A13" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F13" s="2">
-        <v>2073570</v>
       </c>
       <c r="G13" s="2">
         <v>16</v>
@@ -2915,253 +2936,253 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J13" s="3">
-        <f>G13*H13</f>
+        <f t="shared" si="0"/>
         <v>0.128</v>
       </c>
       <c r="K13" s="3">
-        <f>G13*I13</f>
+        <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2073570</v>
+      </c>
+      <c r="G14" s="2">
+        <v>16</v>
+      </c>
+      <c r="H14" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I14" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.128</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>0.128</v>
+      </c>
+      <c r="L14" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="M13" s="14" t="s">
+      <c r="M14" s="13" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A14" s="13" t="s">
+    <row r="15" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G15" s="2">
         <v>12</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H15" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I15" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="J14" s="3">
-        <f>G14*H14</f>
+      <c r="J15" s="3">
+        <f t="shared" si="0"/>
         <v>0.10799999999999998</v>
       </c>
-      <c r="K14" s="3">
-        <f>G14*I14</f>
+      <c r="K15" s="3">
+        <f t="shared" si="1"/>
         <v>0.10799999999999998</v>
       </c>
-      <c r="L14" s="25" t="s">
+      <c r="L15" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="M15" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A15" s="13" t="s">
+    <row r="16" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="2">
         <v>1759083</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G16" s="2">
         <v>16</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H16" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I16" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="J15" s="3">
-        <f>G15*H15</f>
+      <c r="J16" s="3">
+        <f t="shared" si="0"/>
         <v>0.112</v>
       </c>
-      <c r="K15" s="3">
-        <f>G15*I15</f>
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="L16" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="M16" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A16" s="13" t="s">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D17" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <v>1759009</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G17" s="2">
         <v>8</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H17" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I17" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="J16" s="3">
-        <f>G16*H16</f>
+      <c r="J17" s="3">
+        <f t="shared" si="0"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="K16" s="3">
-        <f>G16*I16</f>
+      <c r="K17" s="3">
+        <f t="shared" si="1"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="L16" s="25" t="s">
+      <c r="L17" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M17" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="13" t="s">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A18" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B18" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C18" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F18" s="2">
         <v>8529833</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G18" s="2">
         <v>1</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H18" s="3">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I18" s="3">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="J17" s="3">
-        <f>G17*H17</f>
+      <c r="J18" s="3">
+        <f t="shared" si="0"/>
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="K17" s="3">
-        <f>G17*I17</f>
+      <c r="K18" s="3">
+        <f t="shared" si="1"/>
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="L17" s="42" t="s">
+      <c r="L18" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="M17" s="41" t="s">
+      <c r="M18" s="40" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="13" t="s">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="2">
         <v>1759027</v>
-      </c>
-      <c r="G18" s="2">
-        <v>6</v>
-      </c>
-      <c r="H18" s="3">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="I18" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="J18" s="3">
-        <f>G18*H18</f>
-        <v>5.3999999999999992E-2</v>
-      </c>
-      <c r="K18" s="3">
-        <f>G18*I18</f>
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M18" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="2">
-        <v>2320806</v>
       </c>
       <c r="G19" s="2">
         <v>6</v>
@@ -3173,421 +3194,464 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J19" s="3">
-        <f>G19*H19</f>
+        <f t="shared" si="0"/>
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="K19" s="3">
-        <f>G19*I19</f>
+        <f t="shared" si="1"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="L19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A20" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2320806</v>
+      </c>
+      <c r="G20" s="2">
+        <v>6</v>
+      </c>
+      <c r="H20" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I20" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="0"/>
+        <v>5.3999999999999992E-2</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="1"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M19" s="14" t="s">
+      <c r="M20" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="13" t="s">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A21" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F21" s="2">
         <v>1759037</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G21" s="2">
         <v>5</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H21" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I21" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="J20" s="3">
-        <f>G20*H20</f>
+      <c r="J21" s="3">
+        <f t="shared" si="0"/>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="K20" s="3">
-        <f>G20*I20</f>
+      <c r="K21" s="3">
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="L21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M21" s="13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A21" s="13" t="s">
+    <row r="22" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A22" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F22" s="2">
         <v>2073461</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G22" s="2">
         <v>3</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H22" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I22" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="J21" s="3">
-        <f>G21*H21</f>
+      <c r="J22" s="3">
+        <f t="shared" si="0"/>
         <v>2.4E-2</v>
       </c>
-      <c r="K21" s="3">
-        <f>G21*I21</f>
+      <c r="K22" s="3">
+        <f t="shared" si="1"/>
         <v>2.4E-2</v>
       </c>
-      <c r="L21" s="40" t="s">
+      <c r="L22" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="M22" s="13" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="13" t="s">
+    <row r="23" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A23" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F23" s="2">
         <v>2073388</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G23" s="2">
         <v>1</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H23" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I23" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="J22" s="3">
-        <f>G22*H22</f>
+      <c r="J23" s="3">
+        <f t="shared" si="0"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="K22" s="3">
-        <f>G22*I22</f>
+      <c r="K23" s="3">
+        <f t="shared" si="1"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="L22" s="38" t="s">
+      <c r="L23" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="M22" s="39" t="s">
+      <c r="M23" s="38" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="27" t="s">
+    <row r="24" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A24" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B24" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D24" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E24" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F24" s="27">
         <v>9238760</v>
       </c>
-      <c r="G23" s="28">
+      <c r="G24" s="27">
         <v>1</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H24" s="28">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I23" s="29">
+      <c r="I24" s="28">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J23" s="30">
-        <f>G23*H23</f>
+      <c r="J24" s="29">
+        <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K23" s="30">
-        <f>G23*I23</f>
+      <c r="K24" s="29">
+        <f t="shared" si="1"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L23" s="31" t="s">
+      <c r="L24" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="M23" s="32" t="s">
+      <c r="M24" s="31" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="6" t="s">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A25" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7">
-        <f>SUM(G3:G23)</f>
-        <v>129</v>
-      </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="8">
-        <f>SUM(J3:J23)</f>
-        <v>40.739666666666672</v>
-      </c>
-      <c r="K24" s="8">
-        <f>SUM(K3:K23)</f>
-        <v>23.348333333333336</v>
-      </c>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6">
+        <f>SUM(G3:G24)</f>
+        <v>130</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="7">
+        <f>SUM(J3:J24)</f>
+        <v>40.80466666666667</v>
+      </c>
+      <c r="K25" s="7">
+        <f>SUM(K3:K24)</f>
+        <v>23.375333333333337</v>
+      </c>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
     </row>
     <row r="33" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
     </row>
     <row r="34" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
     </row>
     <row r="35" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
     </row>
     <row r="36" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
     </row>
     <row r="37" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
     </row>
     <row r="38" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
     </row>
     <row r="39" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
     </row>
     <row r="40" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
     </row>
     <row r="41" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
     </row>
     <row r="42" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
     </row>
     <row r="43" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
     </row>
     <row r="44" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
     </row>
     <row r="45" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
     </row>
     <row r="46" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
     </row>
     <row r="47" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
     </row>
     <row r="48" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
     </row>
     <row r="49" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
     </row>
     <row r="50" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
     </row>
     <row r="51" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
     </row>
     <row r="52" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
     </row>
     <row r="53" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
     </row>
     <row r="54" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
     </row>
     <row r="55" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
     </row>
     <row r="56" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
     </row>
     <row r="57" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
     </row>
     <row r="58" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
     </row>
     <row r="59" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
     </row>
     <row r="60" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
     </row>
     <row r="61" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
     </row>
     <row r="62" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
     </row>
     <row r="63" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
     </row>
     <row r="64" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
     </row>
     <row r="65" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
     </row>
     <row r="66" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
     </row>
     <row r="67" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
     </row>
     <row r="68" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
     </row>
     <row r="69" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H69" s="9"/>
-      <c r="I69" s="9"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
     </row>
     <row r="70" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
     </row>
     <row r="71" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
     </row>
     <row r="72" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H72" s="9"/>
-      <c r="I72" s="9"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
     </row>
     <row r="73" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H73" s="9"/>
-      <c r="I73" s="9"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
     </row>
     <row r="74" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
     </row>
     <row r="75" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+    </row>
+    <row r="76" spans="8:9" ht="15.75" customHeight="1">
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3596,46 +3660,47 @@
   <hyperlinks>
     <hyperlink ref="L7" r:id="rId1"/>
     <hyperlink ref="M7" r:id="rId2"/>
-    <hyperlink ref="L15" r:id="rId3"/>
-    <hyperlink ref="M15" r:id="rId4"/>
-    <hyperlink ref="L14" r:id="rId5"/>
-    <hyperlink ref="M14" r:id="rId6"/>
+    <hyperlink ref="L16" r:id="rId3"/>
+    <hyperlink ref="M16" r:id="rId4"/>
+    <hyperlink ref="L15" r:id="rId5"/>
+    <hyperlink ref="M15" r:id="rId6"/>
     <hyperlink ref="L8" r:id="rId7"/>
     <hyperlink ref="M8" r:id="rId8"/>
-    <hyperlink ref="L16" r:id="rId9"/>
-    <hyperlink ref="M16" r:id="rId10"/>
-    <hyperlink ref="L18" r:id="rId11"/>
-    <hyperlink ref="M18" r:id="rId12"/>
-    <hyperlink ref="L19" r:id="rId13"/>
-    <hyperlink ref="M19" r:id="rId14"/>
-    <hyperlink ref="L20" r:id="rId15"/>
-    <hyperlink ref="M20" r:id="rId16"/>
+    <hyperlink ref="L17" r:id="rId9"/>
+    <hyperlink ref="M17" r:id="rId10"/>
+    <hyperlink ref="L19" r:id="rId11"/>
+    <hyperlink ref="M19" r:id="rId12"/>
+    <hyperlink ref="L20" r:id="rId13"/>
+    <hyperlink ref="M20" r:id="rId14"/>
+    <hyperlink ref="L21" r:id="rId15"/>
+    <hyperlink ref="M21" r:id="rId16"/>
     <hyperlink ref="L9" r:id="rId17"/>
     <hyperlink ref="M9" r:id="rId18"/>
     <hyperlink ref="L10" r:id="rId19"/>
-    <hyperlink ref="L11" r:id="rId20"/>
-    <hyperlink ref="M11" r:id="rId21"/>
-    <hyperlink ref="L3" r:id="rId22"/>
-    <hyperlink ref="M3" r:id="rId23"/>
-    <hyperlink ref="L4" r:id="rId24"/>
-    <hyperlink ref="M4" r:id="rId25"/>
-    <hyperlink ref="L5" r:id="rId26"/>
-    <hyperlink ref="M5" r:id="rId27"/>
-    <hyperlink ref="E6" r:id="rId28"/>
-    <hyperlink ref="L6" r:id="rId29"/>
-    <hyperlink ref="L12" r:id="rId30"/>
-    <hyperlink ref="M12" r:id="rId31"/>
-    <hyperlink ref="L13" r:id="rId32"/>
-    <hyperlink ref="M13" r:id="rId33"/>
-    <hyperlink ref="L21" r:id="rId34"/>
-    <hyperlink ref="M21" r:id="rId35"/>
-    <hyperlink ref="L23" r:id="rId36"/>
-    <hyperlink ref="M23" r:id="rId37"/>
+    <hyperlink ref="M12" r:id="rId20"/>
+    <hyperlink ref="L3" r:id="rId21"/>
+    <hyperlink ref="M3" r:id="rId22"/>
+    <hyperlink ref="L4" r:id="rId23"/>
+    <hyperlink ref="M4" r:id="rId24"/>
+    <hyperlink ref="L5" r:id="rId25"/>
+    <hyperlink ref="M5" r:id="rId26"/>
+    <hyperlink ref="E6" r:id="rId27"/>
+    <hyperlink ref="L6" r:id="rId28"/>
+    <hyperlink ref="L13" r:id="rId29"/>
+    <hyperlink ref="M13" r:id="rId30"/>
+    <hyperlink ref="L14" r:id="rId31"/>
+    <hyperlink ref="M14" r:id="rId32"/>
+    <hyperlink ref="L22" r:id="rId33"/>
+    <hyperlink ref="M22" r:id="rId34"/>
+    <hyperlink ref="L24" r:id="rId35"/>
+    <hyperlink ref="M24" r:id="rId36"/>
+    <hyperlink ref="L12" r:id="rId37"/>
+    <hyperlink ref="M11" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId39"/>
   <tableParts count="1">
-    <tablePart r:id="rId39"/>
+    <tablePart r:id="rId40"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3653,10 +3718,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix olimex header genre to female
The two Olimex 2x20 pins 1.27" pitch has been changed from male to
female.
</commit_message>
<xml_diff>
--- a/hardware/eagle/bom.xlsx
+++ b/hardware/eagle/bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="159">
   <si>
     <t>category</t>
   </si>
@@ -255,24 +255,12 @@
     <t>connector</t>
   </si>
   <si>
-    <t>0.05" male SMD 2x20</t>
-  </si>
-  <si>
     <t>OLIMEX</t>
   </si>
   <si>
-    <t>MALE-PAV16X-2x20</t>
-  </si>
-  <si>
     <t>OLIMEX</t>
   </si>
   <si>
-    <t>MALE-PAV16X-2x20</t>
-  </si>
-  <si>
-    <t>https://www.olimex.com/Products/Components/Connectors/MALE-PAV16X-2x20/</t>
-  </si>
-  <si>
     <t>connector</t>
   </si>
   <si>
@@ -499,6 +487,15 @@
   </si>
   <si>
     <t>http://www.farnell.com/datasheets/1518407.pdf</t>
+  </si>
+  <si>
+    <t>0.05" female SMD 2x20</t>
+  </si>
+  <si>
+    <t>https://www.olimex.com/Products/Components/Connectors/FEMALE-YAV36P-2x20/</t>
+  </si>
+  <si>
+    <t>FEMALE-YAV36P-2x20</t>
   </si>
 </sst>
 </file>
@@ -509,7 +506,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -542,10 +539,6 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -934,7 +927,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -945,16 +938,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="14" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -963,35 +956,33 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2391,9 +2382,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2401,9 +2392,9 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.85546875" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
@@ -2414,19 +2405,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18">
-      <c r="A1" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
+      <c r="A1" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1">
       <c r="A2" s="15" t="s">
@@ -2489,19 +2480,19 @@
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
       <c r="A3" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="F3" s="2">
         <v>1882283</v>
@@ -2523,28 +2514,28 @@
         <f t="shared" ref="K3:K24" si="1">G3*I3</f>
         <v>10.41</v>
       </c>
-      <c r="L3" s="25" t="s">
-        <v>96</v>
+      <c r="L3" s="24" t="s">
+        <v>92</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1">
       <c r="A4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="F4" s="2">
         <v>1689419</v>
@@ -2566,28 +2557,28 @@
         <f t="shared" si="1"/>
         <v>5.83</v>
       </c>
-      <c r="L4" s="25" t="s">
-        <v>103</v>
+      <c r="L4" s="24" t="s">
+        <v>99</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1">
       <c r="A5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="F5" s="2">
         <v>9306803</v>
@@ -2609,22 +2600,22 @@
         <f t="shared" si="1"/>
         <v>1.51</v>
       </c>
-      <c r="L5" s="25" t="s">
-        <v>110</v>
+      <c r="L5" s="24" t="s">
+        <v>106</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
+        <v>108</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="2"/>
       <c r="E6" s="21" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
@@ -2647,7 +2638,7 @@
         <v>1.1893333333333334</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M6" s="14"/>
     </row>
@@ -2773,66 +2764,66 @@
         <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
-      <c r="L9" s="25" t="s">
+      <c r="L9" s="24" t="s">
         <v>75</v>
       </c>
       <c r="M9" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="15.75" customHeight="1">
+    <row r="10" spans="1:31" s="41" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="12" t="s">
         <v>77</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="D10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>82</v>
+      <c r="F10" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="G10" s="2">
         <v>2</v>
       </c>
       <c r="H10" s="3">
-        <v>0.36</v>
+        <v>0.4</v>
       </c>
       <c r="I10" s="3">
         <v>0.32</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
-      <c r="L10" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:31" s="36" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L10" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="M10" s="13"/>
+    </row>
+    <row r="11" spans="1:31" s="35" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="12" t="s">
         <v>70</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>17</v>
@@ -2857,28 +2848,28 @@
         <f t="shared" ref="K11" si="3">G11*I11</f>
         <v>2.7E-2</v>
       </c>
-      <c r="L11" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="M11" s="45" t="s">
-        <v>159</v>
+      <c r="L11" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="M11" s="43" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1">
       <c r="A12" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="F12" s="2">
         <v>1593440</v>
@@ -2900,28 +2891,28 @@
         <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
-      <c r="L12" s="44" t="s">
-        <v>89</v>
+      <c r="L12" s="42" t="s">
+        <v>85</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1">
       <c r="A13" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>115</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>119</v>
       </c>
       <c r="F13" s="22">
         <v>2073537</v>
@@ -2943,28 +2934,28 @@
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="L13" s="24" t="s">
-        <v>120</v>
+      <c r="L13" s="23" t="s">
+        <v>116</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1">
       <c r="A14" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="F14" s="2">
         <v>2073570</v>
@@ -2986,11 +2977,11 @@
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="L14" s="24" t="s">
-        <v>127</v>
+      <c r="L14" s="23" t="s">
+        <v>123</v>
       </c>
       <c r="M14" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1">
@@ -3029,7 +3020,7 @@
         <f t="shared" si="1"/>
         <v>0.10799999999999998</v>
       </c>
-      <c r="L15" s="24" t="s">
+      <c r="L15" s="23" t="s">
         <v>33</v>
       </c>
       <c r="M15" s="13" t="s">
@@ -3072,7 +3063,7 @@
         <f t="shared" si="1"/>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="L16" s="24" t="s">
+      <c r="L16" s="23" t="s">
         <v>25</v>
       </c>
       <c r="M16" s="13" t="s">
@@ -3089,7 +3080,7 @@
       <c r="C17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="33" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -3115,7 +3106,7 @@
         <f t="shared" si="1"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="L17" s="24" t="s">
+      <c r="L17" s="23" t="s">
         <v>47</v>
       </c>
       <c r="M17" s="13" t="s">
@@ -3124,16 +3115,16 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>151</v>
+        <v>145</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>147</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>17</v>
@@ -3158,11 +3149,11 @@
         <f t="shared" si="1"/>
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="L18" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="M18" s="40" t="s">
-        <v>154</v>
+      <c r="L18" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="M18" s="39" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
@@ -3296,19 +3287,19 @@
     </row>
     <row r="22" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="F22" s="2">
         <v>2073461</v>
@@ -3330,25 +3321,25 @@
         <f t="shared" si="1"/>
         <v>2.4E-2</v>
       </c>
-      <c r="L22" s="39" t="s">
-        <v>134</v>
+      <c r="L22" s="38" t="s">
+        <v>130</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>17</v>
@@ -3373,59 +3364,59 @@
         <f t="shared" si="1"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="L23" s="37" t="s">
-        <v>147</v>
-      </c>
-      <c r="M23" s="38" t="s">
-        <v>121</v>
+      <c r="L23" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="M23" s="37" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="B24" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="F24" s="27">
+      <c r="F24" s="26">
         <v>9238760</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="26">
         <v>1</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="27">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I24" s="28">
+      <c r="I24" s="27">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J24" s="29">
+      <c r="J24" s="28">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K24" s="29">
+      <c r="K24" s="28">
         <f t="shared" si="1"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L24" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="M24" s="31" t="s">
-        <v>142</v>
+      <c r="L24" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="M24" s="30" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
@@ -3440,7 +3431,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="7">
         <f>SUM(J3:J24)</f>
-        <v>40.80466666666667</v>
+        <v>40.884666666666668</v>
       </c>
       <c r="K25" s="7">
         <f>SUM(K3:K24)</f>
@@ -3719,10 +3710,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed BOM capacitor reference
removed the Tape & Reel service, which has a 100+ minimun order number.
</commit_message>
<xml_diff>
--- a/hardware/eagle/bom.xlsx
+++ b/hardware/eagle/bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="158">
   <si>
     <t>category</t>
   </si>
@@ -117,12 +117,6 @@
     <t>Farnell</t>
   </si>
   <si>
-    <t>1759398RL</t>
-  </si>
-  <si>
-    <t>http://fr.farnell.com/multicomp/mcca000521/condensateur-mlcc-06035v-10v-1uf/dp/1759398RL</t>
-  </si>
-  <si>
     <t>http://www.farnell.com/datasheets/1723208.pdf</t>
   </si>
   <si>
@@ -496,6 +490,9 @@
   </si>
   <si>
     <t>FEMALE-YAV36P-2x20</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/multicomp/mcca000521/condensateur-mlcc-06035v-10v-1uf/dp/1759398</t>
   </si>
 </sst>
 </file>
@@ -951,12 +948,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -966,10 +959,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -983,6 +972,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2069,8 +2066,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A2:M24" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A2:M24"/>
-  <sortState ref="A3:M23">
-    <sortCondition descending="1" ref="K2:K23"/>
+  <sortState ref="A3:M24">
+    <sortCondition ref="A2:A24"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" name="category" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
@@ -2382,9 +2379,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2405,19 +2402,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18">
-      <c r="A1" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="A1" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1">
       <c r="A2" s="15" t="s">
@@ -2480,826 +2477,826 @@
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2">
-        <v>1882283</v>
+        <v>2254444</v>
       </c>
       <c r="G3" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H3" s="3">
-        <v>4.88</v>
+        <v>0.41</v>
       </c>
       <c r="I3" s="3">
-        <v>3.47</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="J3" s="3">
-        <f t="shared" ref="J3:J24" si="0">G3*H3</f>
-        <v>14.64</v>
+        <f>G3*H3</f>
+        <v>2.8699999999999997</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K24" si="1">G3*I3</f>
-        <v>10.41</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>92</v>
+        <f>G3*I3</f>
+        <v>1.036</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="F4" s="2">
-        <v>1689419</v>
+        <v>1759136</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="H4" s="3">
-        <v>11.86</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="I4" s="3">
-        <v>5.83</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" si="0"/>
-        <v>11.86</v>
+        <f>G4*H4</f>
+        <v>1.008</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="1"/>
-        <v>5.83</v>
-      </c>
-      <c r="L4" s="24" t="s">
-        <v>99</v>
+        <f>G4*I4</f>
+        <v>1.008</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>100</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>104</v>
+        <v>29</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2">
-        <v>9306803</v>
+        <v>1759398</v>
       </c>
       <c r="G5" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H5" s="3">
-        <v>1.7</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="I5" s="3">
-        <v>1.51</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="0"/>
-        <v>1.7</v>
+        <f>G5*H5</f>
+        <v>0.10799999999999998</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="1"/>
-        <v>1.51</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>106</v>
+        <f>G5*I5</f>
+        <v>0.10799999999999998</v>
+      </c>
+      <c r="L5" s="45" t="s">
+        <v>157</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>107</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1759083</v>
+      </c>
       <c r="G6" s="2">
+        <v>16</v>
+      </c>
+      <c r="H6" s="3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I6" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J6" s="3">
+        <f>G6*H6</f>
+        <v>0.112</v>
+      </c>
+      <c r="K6" s="3">
+        <f>G6*I6</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1759009</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8</v>
+      </c>
+      <c r="H7" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="J7" s="3">
+        <f>G7*H7</f>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="K7" s="3">
+        <f>G7*I7</f>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1759027</v>
+      </c>
+      <c r="G8" s="2">
+        <v>6</v>
+      </c>
+      <c r="H8" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I8" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J8" s="3">
+        <f>G8*H8</f>
+        <v>5.3999999999999992E-2</v>
+      </c>
+      <c r="K8" s="3">
+        <f>G8*I8</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2320806</v>
+      </c>
+      <c r="G9" s="2">
+        <v>6</v>
+      </c>
+      <c r="H9" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I9" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J9" s="3">
+        <f>G9*H9</f>
+        <v>5.3999999999999992E-2</v>
+      </c>
+      <c r="K9" s="3">
+        <f>G9*I9</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" s="35" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1759037</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I10" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J10" s="3">
+        <f>G10*H10</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="K10" s="3">
+        <f>G10*I10</f>
+        <v>0.03</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" s="29" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A11" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="19">
+        <v>1593445</v>
+      </c>
+      <c r="G11" s="2">
         <v>1</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H11" s="3">
+        <v>0.83</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="J11" s="3">
+        <f>G11*H11</f>
+        <v>0.83</v>
+      </c>
+      <c r="K11" s="3">
+        <f>G11*I11</f>
+        <v>0.64</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A12" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="J12" s="3">
+        <f>G12*H12</f>
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="3">
+        <f>G12*I12</f>
+        <v>0.64</v>
+      </c>
+      <c r="L12" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="M12" s="13"/>
+    </row>
+    <row r="13" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="19">
+        <v>1593411</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="J13" s="3">
+        <f>G13*H13</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="K13" s="3">
+        <f>G13*I13</f>
+        <v>2.7E-2</v>
+      </c>
+      <c r="L13" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="M13" s="37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1593440</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="J14" s="3">
+        <f>G14*H14</f>
+        <v>0.36</v>
+      </c>
+      <c r="K14" s="3">
+        <f>G14*I14</f>
+        <v>0.32</v>
+      </c>
+      <c r="L14" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1882283</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3">
+        <v>4.88</v>
+      </c>
+      <c r="I15" s="3">
+        <v>3.47</v>
+      </c>
+      <c r="J15" s="3">
+        <f>G15*H15</f>
+        <v>14.64</v>
+      </c>
+      <c r="K15" s="3">
+        <f>G15*I15</f>
+        <v>10.41</v>
+      </c>
+      <c r="L15" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1689419</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>11.86</v>
+      </c>
+      <c r="I16" s="3">
+        <v>5.83</v>
+      </c>
+      <c r="J16" s="3">
+        <f>G16*H16</f>
+        <v>11.86</v>
+      </c>
+      <c r="K16" s="3">
+        <f>G16*I16</f>
+        <v>5.83</v>
+      </c>
+      <c r="L16" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A17" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="2">
+        <v>9306803</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1.51</v>
+      </c>
+      <c r="J17" s="3">
+        <f>G17*H17</f>
+        <v>1.7</v>
+      </c>
+      <c r="K17" s="3">
+        <f>G17*I17</f>
+        <v>1.51</v>
+      </c>
+      <c r="L17" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A18" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="2">
+        <v>8529833</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="I18" s="3">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="J18" s="3">
+        <f>G18*H18</f>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="K18" s="3">
+        <f>G18*I18</f>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="L18" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="M18" s="33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
         <f>17.84/3</f>
         <v>5.9466666666666663</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I19" s="3">
         <f>Tableau3[[#This Row],[€ / u / 1pc]]/5</f>
         <v>1.1893333333333334</v>
       </c>
-      <c r="J6" s="3">
-        <f t="shared" si="0"/>
+      <c r="J19" s="3">
+        <f>G19*H19</f>
         <v>5.9466666666666663</v>
       </c>
-      <c r="K6" s="3">
-        <f t="shared" si="1"/>
+      <c r="K19" s="3">
+        <f>G19*I19</f>
         <v>1.1893333333333334</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2254444</v>
-      </c>
-      <c r="G7" s="2">
-        <v>7</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.41</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="J7" s="3">
-        <f t="shared" si="0"/>
-        <v>2.8699999999999997</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="1"/>
-        <v>1.036</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1759136</v>
-      </c>
-      <c r="G8" s="2">
-        <v>21</v>
-      </c>
-      <c r="H8" s="3">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="I8" s="3">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="J8" s="3">
-        <f t="shared" si="0"/>
-        <v>1.008</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" si="1"/>
-        <v>1.008</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A9" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1593445</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0.83</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0.64</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="0"/>
-        <v>0.83</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="1"/>
-        <v>0.64</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" s="41" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G10" s="2">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" si="1"/>
-        <v>0.64</v>
-      </c>
-      <c r="L10" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="M10" s="13"/>
-    </row>
-    <row r="11" spans="1:31" s="35" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="22">
-        <v>1593411</v>
-      </c>
-      <c r="G11" s="2">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="I11" s="3">
-        <v>2.7E-2</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" ref="J11" si="2">G11*H11</f>
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="K11" s="3">
-        <f t="shared" ref="K11" si="3">G11*I11</f>
-        <v>2.7E-2</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="M11" s="43" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A12" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1593440</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.36</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="0"/>
-        <v>0.36</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" si="1"/>
-        <v>0.32</v>
-      </c>
-      <c r="L12" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A13" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="F13" s="22">
-        <v>2073537</v>
-      </c>
-      <c r="G13" s="2">
-        <v>16</v>
-      </c>
-      <c r="H13" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I13" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="J13" s="3">
-        <f t="shared" si="0"/>
-        <v>0.128</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" si="1"/>
-        <v>0.128</v>
-      </c>
-      <c r="L13" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A14" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F14" s="2">
-        <v>2073570</v>
-      </c>
-      <c r="G14" s="2">
-        <v>16</v>
-      </c>
-      <c r="H14" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I14" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="J14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.128</v>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" si="1"/>
-        <v>0.128</v>
-      </c>
-      <c r="L14" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A15" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="2">
-        <v>12</v>
-      </c>
-      <c r="H15" s="3">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="I15" s="3">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="J15" s="3">
-        <f t="shared" si="0"/>
-        <v>0.10799999999999998</v>
-      </c>
-      <c r="K15" s="3">
-        <f t="shared" si="1"/>
-        <v>0.10799999999999998</v>
-      </c>
-      <c r="L15" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="M15" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1759083</v>
-      </c>
-      <c r="G16" s="2">
-        <v>16</v>
-      </c>
-      <c r="H16" s="3">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="I16" s="3">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="J16" s="3">
-        <f t="shared" si="0"/>
-        <v>0.112</v>
-      </c>
-      <c r="K16" s="3">
-        <f t="shared" si="1"/>
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="L16" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1759009</v>
-      </c>
-      <c r="G17" s="2">
-        <v>8</v>
-      </c>
-      <c r="H17" s="3">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="I17" s="3">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="J17" s="3">
-        <f t="shared" si="0"/>
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" si="1"/>
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="L17" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="2">
-        <v>8529833</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="I18" s="3">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="J18" s="3">
-        <f t="shared" si="0"/>
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="K18" s="3">
-        <f t="shared" si="1"/>
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="L18" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="M18" s="39" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1759027</v>
-      </c>
-      <c r="G19" s="2">
-        <v>6</v>
-      </c>
-      <c r="H19" s="3">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="I19" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="J19" s="3">
-        <f t="shared" si="0"/>
-        <v>5.3999999999999992E-2</v>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" si="1"/>
-        <v>4.8000000000000001E-2</v>
-      </c>
       <c r="L19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>55</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="M19" s="14"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="12" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="F20" s="2">
-        <v>2320806</v>
+        <v>2073537</v>
       </c>
       <c r="G20" s="2">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H20" s="3">
-        <v>8.9999999999999993E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="I20" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="0"/>
-        <v>5.3999999999999992E-2</v>
+        <f>G20*H20</f>
+        <v>0.128</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" si="1"/>
-        <v>4.8000000000000001E-2</v>
+        <f>G20*I20</f>
+        <v>0.128</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="M20" s="13" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="12" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>67</v>
+        <v>120</v>
       </c>
       <c r="F21" s="2">
-        <v>1759037</v>
+        <v>2073570</v>
       </c>
       <c r="G21" s="2">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H21" s="3">
-        <v>7.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="I21" s="3">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
+        <f>G21*H21</f>
+        <v>0.128</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="1"/>
-        <v>0.03</v>
+        <f>G21*I21</f>
+        <v>0.128</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="F22" s="2">
         <v>2073461</v>
@@ -3314,32 +3311,32 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="0"/>
+        <f>G22*H22</f>
         <v>2.4E-2</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="1"/>
+        <f>G22*I22</f>
         <v>2.4E-2</v>
       </c>
-      <c r="L22" s="38" t="s">
-        <v>130</v>
+      <c r="L22" s="32" t="s">
+        <v>128</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>17</v>
@@ -3357,66 +3354,66 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="0"/>
+        <f>G23*H23</f>
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="K23" s="3">
-        <f t="shared" si="1"/>
+        <f>G23*I23</f>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="L23" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="M23" s="37" t="s">
-        <v>117</v>
+      <c r="L23" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="M23" s="31" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="D24" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="E24" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="F24" s="22">
+        <v>9238760</v>
+      </c>
+      <c r="G24" s="22">
+        <v>1</v>
+      </c>
+      <c r="H24" s="23">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I24" s="23">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J24" s="24">
+        <f>G24*H24</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K24" s="24">
+        <f>G24*I24</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L24" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="M24" s="26" t="s">
         <v>136</v>
-      </c>
-      <c r="F24" s="26">
-        <v>9238760</v>
-      </c>
-      <c r="G24" s="26">
-        <v>1</v>
-      </c>
-      <c r="H24" s="27">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="I24" s="27">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="J24" s="28">
-        <f t="shared" si="0"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="K24" s="28">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="L24" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="M24" s="30" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
@@ -3431,7 +3428,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="7">
         <f>SUM(J3:J24)</f>
-        <v>40.884666666666668</v>
+        <v>40.884666666666675</v>
       </c>
       <c r="K25" s="7">
         <f>SUM(K3:K24)</f>
@@ -3649,49 +3646,48 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L7" r:id="rId1"/>
-    <hyperlink ref="M7" r:id="rId2"/>
-    <hyperlink ref="L16" r:id="rId3"/>
-    <hyperlink ref="M16" r:id="rId4"/>
-    <hyperlink ref="L15" r:id="rId5"/>
-    <hyperlink ref="M15" r:id="rId6"/>
-    <hyperlink ref="L8" r:id="rId7"/>
-    <hyperlink ref="M8" r:id="rId8"/>
-    <hyperlink ref="L17" r:id="rId9"/>
-    <hyperlink ref="M17" r:id="rId10"/>
-    <hyperlink ref="L19" r:id="rId11"/>
-    <hyperlink ref="M19" r:id="rId12"/>
-    <hyperlink ref="L20" r:id="rId13"/>
-    <hyperlink ref="M20" r:id="rId14"/>
-    <hyperlink ref="L21" r:id="rId15"/>
-    <hyperlink ref="M21" r:id="rId16"/>
-    <hyperlink ref="L9" r:id="rId17"/>
-    <hyperlink ref="M9" r:id="rId18"/>
-    <hyperlink ref="L10" r:id="rId19"/>
-    <hyperlink ref="M12" r:id="rId20"/>
-    <hyperlink ref="L3" r:id="rId21"/>
-    <hyperlink ref="M3" r:id="rId22"/>
-    <hyperlink ref="L4" r:id="rId23"/>
-    <hyperlink ref="M4" r:id="rId24"/>
-    <hyperlink ref="L5" r:id="rId25"/>
-    <hyperlink ref="M5" r:id="rId26"/>
-    <hyperlink ref="E6" r:id="rId27"/>
-    <hyperlink ref="L6" r:id="rId28"/>
-    <hyperlink ref="L13" r:id="rId29"/>
-    <hyperlink ref="M13" r:id="rId30"/>
-    <hyperlink ref="L14" r:id="rId31"/>
-    <hyperlink ref="M14" r:id="rId32"/>
-    <hyperlink ref="L22" r:id="rId33"/>
-    <hyperlink ref="M22" r:id="rId34"/>
-    <hyperlink ref="L24" r:id="rId35"/>
-    <hyperlink ref="M24" r:id="rId36"/>
-    <hyperlink ref="L12" r:id="rId37"/>
-    <hyperlink ref="M11" r:id="rId38"/>
+    <hyperlink ref="L3" r:id="rId1"/>
+    <hyperlink ref="M3" r:id="rId2"/>
+    <hyperlink ref="L6" r:id="rId3"/>
+    <hyperlink ref="M6" r:id="rId4"/>
+    <hyperlink ref="L5" r:id="rId5"/>
+    <hyperlink ref="M5" r:id="rId6"/>
+    <hyperlink ref="L4" r:id="rId7"/>
+    <hyperlink ref="M4" r:id="rId8"/>
+    <hyperlink ref="L7" r:id="rId9"/>
+    <hyperlink ref="M7" r:id="rId10"/>
+    <hyperlink ref="L8" r:id="rId11"/>
+    <hyperlink ref="M8" r:id="rId12"/>
+    <hyperlink ref="L9" r:id="rId13"/>
+    <hyperlink ref="M9" r:id="rId14"/>
+    <hyperlink ref="L10" r:id="rId15"/>
+    <hyperlink ref="M10" r:id="rId16"/>
+    <hyperlink ref="L11" r:id="rId17"/>
+    <hyperlink ref="M11" r:id="rId18"/>
+    <hyperlink ref="L12" r:id="rId19"/>
+    <hyperlink ref="M14" r:id="rId20"/>
+    <hyperlink ref="L15" r:id="rId21"/>
+    <hyperlink ref="M15" r:id="rId22"/>
+    <hyperlink ref="L16" r:id="rId23"/>
+    <hyperlink ref="M16" r:id="rId24"/>
+    <hyperlink ref="L17" r:id="rId25"/>
+    <hyperlink ref="M17" r:id="rId26"/>
+    <hyperlink ref="L19" r:id="rId27"/>
+    <hyperlink ref="L20" r:id="rId28"/>
+    <hyperlink ref="M20" r:id="rId29"/>
+    <hyperlink ref="L21" r:id="rId30"/>
+    <hyperlink ref="M21" r:id="rId31"/>
+    <hyperlink ref="L22" r:id="rId32"/>
+    <hyperlink ref="M22" r:id="rId33"/>
+    <hyperlink ref="L24" r:id="rId34"/>
+    <hyperlink ref="M24" r:id="rId35"/>
+    <hyperlink ref="L14" r:id="rId36"/>
+    <hyperlink ref="M13" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId39"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
   <tableParts count="1">
-    <tablePart r:id="rId40"/>
+    <tablePart r:id="rId39"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3710,10 +3706,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed BOM taxes issues
fix #5

Order in US Dollars are converted in Euros.
French Taxes (VAT) is added in grand total.
</commit_message>
<xml_diff>
--- a/hardware/eagle/bom.xlsx
+++ b/hardware/eagle/bom.xlsx
@@ -11,7 +11,7 @@
     <sheet name="other" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$2:$M$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$3:$M$25</definedName>
     <definedName name="PlageNommée1">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="165">
   <si>
     <t>category</t>
   </si>
@@ -493,17 +493,39 @@
   </si>
   <si>
     <t>http://fr.farnell.com/multicomp/mcca000521/condensateur-mlcc-06035v-10v-1uf/dp/1759398</t>
+  </si>
+  <si>
+    <t>taxe rate =</t>
+  </si>
+  <si>
+    <t>1 € =</t>
+  </si>
+  <si>
+    <t>taxes excluded</t>
+  </si>
+  <si>
+    <t>taxes</t>
+  </si>
+  <si>
+    <t>grand total</t>
+  </si>
+  <si>
+    <t>France VAT</t>
+  </si>
+  <si>
+    <t>for the pcb (order in $)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1]"/>
+    <numFmt numFmtId="176" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -609,8 +631,37 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -634,18 +685,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF3D85C6"/>
+        <bgColor rgb="FF3D85C6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3D85C6"/>
-        <bgColor rgb="FF3D85C6"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -921,71 +990,177 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="23" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="24" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="25" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="25" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1017,45 +1192,9 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1091,7 +1230,9 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1103,13 +1244,14 @@
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color rgb="FF0000FF"/>
+        <color auto="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1117,7 +1259,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1130,8 +1272,123 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1167,48 +1424,9 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1244,48 +1462,9 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1321,48 +1500,9 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1398,48 +1538,9 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1475,47 +1576,9 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1551,351 +1614,9 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1929,45 +1650,9 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1979,46 +1664,22 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -2064,29 +1725,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A2:M24" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="A2:M24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A3:M25" headerRowDxfId="17" dataDxfId="0" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+  <autoFilter ref="A3:M25"/>
   <sortState ref="A3:M24">
     <sortCondition ref="A2:A24"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="category" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" name="value/description" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" name="manufacturer name" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="manufacturer ref" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="vendor name" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="vendor ref" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="7" name="qty" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="8" name="€ / u / 1pc" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="9" name="€ / u / 100pcs" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="10" name="€ / 1pc" dataDxfId="7" totalsRowDxfId="6">
-      <calculatedColumnFormula>G3*H3</calculatedColumnFormula>
+    <tableColumn id="1" name="category" totalsRowLabel="Total" dataDxfId="13"/>
+    <tableColumn id="2" name="value/description" dataDxfId="12"/>
+    <tableColumn id="3" name="manufacturer name" dataDxfId="11"/>
+    <tableColumn id="4" name="manufacturer ref" dataDxfId="10"/>
+    <tableColumn id="5" name="vendor name" dataDxfId="9"/>
+    <tableColumn id="6" name="vendor ref" dataDxfId="8"/>
+    <tableColumn id="7" name="qty" dataDxfId="7"/>
+    <tableColumn id="8" name="€ / u / 1pc" dataDxfId="6"/>
+    <tableColumn id="9" name="€ / u / 100pcs" dataDxfId="5"/>
+    <tableColumn id="10" name="€ / 1pc" dataDxfId="4">
+      <calculatedColumnFormula>G4*H4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="€ / 100pc" dataDxfId="5" totalsRowDxfId="4">
-      <calculatedColumnFormula>G3*I3</calculatedColumnFormula>
+    <tableColumn id="11" name="€ / 100pc" dataDxfId="3">
+      <calculatedColumnFormula>G4*I4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="link" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="13" name="datasheet" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="12" name="link" dataDxfId="2"/>
+    <tableColumn id="13" name="datasheet" totalsRowFunction="count" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2377,11 +2038,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE76"/>
+  <dimension ref="A1:AE77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2402,1287 +2063,1345 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-    </row>
-    <row r="2" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+    </row>
+    <row r="2" spans="1:31" s="16" customFormat="1" ht="18.75">
+      <c r="A2" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+    </row>
+    <row r="3" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-    </row>
-    <row r="3" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+    </row>
+    <row r="4" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F4" s="21">
         <v>2254444</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G4" s="21">
         <v>7</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H4" s="22">
         <v>0.41</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I4" s="22">
         <v>0.14799999999999999</v>
       </c>
-      <c r="J3" s="3">
-        <f>G3*H3</f>
+      <c r="J4" s="22">
+        <f>G4*H4</f>
         <v>2.8699999999999997</v>
       </c>
-      <c r="K3" s="3">
-        <f>G3*I3</f>
+      <c r="K4" s="22">
+        <f>G4*I4</f>
         <v>1.036</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M4" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A4" s="12" t="s">
+    <row r="5" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="21">
         <v>1759136</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G5" s="21">
         <v>21</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H5" s="22">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I5" s="22">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="J4" s="3">
-        <f>G4*H4</f>
+      <c r="J5" s="22">
+        <f>G5*H5</f>
         <v>1.008</v>
       </c>
-      <c r="K4" s="3">
-        <f>G4*I4</f>
+      <c r="K5" s="22">
+        <f>G5*I5</f>
         <v>1.008</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L5" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M5" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A5" s="12" t="s">
+    <row r="6" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F6" s="21">
         <v>1759398</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G6" s="21">
         <v>12</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H6" s="22">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I6" s="22">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="J5" s="3">
-        <f>G5*H5</f>
+      <c r="J6" s="22">
+        <f>G6*H6</f>
         <v>0.10799999999999998</v>
       </c>
-      <c r="K5" s="3">
-        <f>G5*I5</f>
+      <c r="K6" s="22">
+        <f>G6*I6</f>
         <v>0.10799999999999998</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="L6" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="M6" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A6" s="12" t="s">
+    <row r="7" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E7" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F7" s="21">
         <v>1759083</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G7" s="21">
         <v>16</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H7" s="22">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I7" s="22">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="J6" s="3">
-        <f>G6*H6</f>
+      <c r="J7" s="22">
+        <f>G7*H7</f>
         <v>0.112</v>
       </c>
-      <c r="K6" s="3">
-        <f>G6*I6</f>
+      <c r="K7" s="22">
+        <f>G7*I7</f>
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M7" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A7" s="12" t="s">
+    <row r="8" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A8" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="21">
         <v>1759009</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G8" s="21">
         <v>8</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H8" s="22">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I8" s="22">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="J7" s="3">
-        <f>G7*H7</f>
+      <c r="J8" s="22">
+        <f>G8*H8</f>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="K7" s="3">
-        <f>G7*I7</f>
+      <c r="K8" s="22">
+        <f>G8*I8</f>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L8" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M8" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A8" s="12" t="s">
+    <row r="9" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A9" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="21">
         <v>1759027</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="21">
         <v>6</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H9" s="22">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I9" s="22">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="J8" s="3">
-        <f>G8*H8</f>
-        <v>5.3999999999999992E-2</v>
-      </c>
-      <c r="K8" s="3">
-        <f>G8*I8</f>
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A9" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="2">
-        <v>2320806</v>
-      </c>
-      <c r="G9" s="2">
-        <v>6</v>
-      </c>
-      <c r="H9" s="3">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="I9" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="J9" s="3">
+      <c r="J9" s="22">
         <f>G9*H9</f>
         <v>5.3999999999999992E-2</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="22">
         <f>G9*I9</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A10" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="21">
+        <v>2320806</v>
+      </c>
+      <c r="G10" s="21">
+        <v>6</v>
+      </c>
+      <c r="H10" s="22">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I10" s="22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J10" s="22">
+        <f>G10*H10</f>
+        <v>5.3999999999999992E-2</v>
+      </c>
+      <c r="K10" s="22">
+        <f>G10*I10</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L10" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="M10" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:31" s="35" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="12" t="s">
+    <row r="11" spans="1:31" s="16" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A11" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="21">
         <v>1759037</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G11" s="21">
         <v>5</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H11" s="22">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I11" s="22">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="J10" s="3">
-        <f>G10*H10</f>
+      <c r="J11" s="22">
+        <f>G11*H11</f>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="K10" s="3">
-        <f>G10*I10</f>
+      <c r="K11" s="22">
+        <f>G11*I11</f>
         <v>0.03</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L11" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="M11" s="13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:31" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="12" t="s">
+    <row r="12" spans="1:31" s="11" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A12" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F12" s="26">
         <v>1593445</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="21">
         <v>1</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H12" s="22">
         <v>0.83</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I12" s="22">
         <v>0.64</v>
       </c>
-      <c r="J11" s="3">
-        <f>G11*H11</f>
+      <c r="J12" s="22">
+        <f>G12*H12</f>
         <v>0.83</v>
       </c>
-      <c r="K11" s="3">
-        <f>G11*I11</f>
-        <v>0.64</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A12" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="J12" s="3">
-        <f>G12*H12</f>
-        <v>0.8</v>
-      </c>
-      <c r="K12" s="3">
+      <c r="K12" s="22">
         <f>G12*I12</f>
         <v>0.64</v>
       </c>
-      <c r="L12" s="44" t="s">
+      <c r="L12" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A13" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="G13" s="21">
+        <v>2</v>
+      </c>
+      <c r="H13" s="28">
+        <f>0.4*(1-$B$27)</f>
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="I13" s="22">
+        <f>0.32*(1-$B$27)</f>
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="J13" s="22">
+        <f>G13*H13</f>
+        <v>0.64000000000000012</v>
+      </c>
+      <c r="K13" s="22">
+        <f>G13*I13</f>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="L13" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="M12" s="13"/>
-    </row>
-    <row r="13" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A13" s="12" t="s">
+      <c r="M13" s="13"/>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A14" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C14" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D14" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E14" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F14" s="26">
         <v>1593411</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G14" s="21">
         <v>1</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H14" s="22">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I14" s="22">
         <v>2.7E-2</v>
       </c>
-      <c r="J13" s="3">
-        <f>G13*H13</f>
+      <c r="J14" s="22">
+        <f>G14*H14</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="K13" s="3">
-        <f>G13*I13</f>
+      <c r="K14" s="22">
+        <f>G14*I14</f>
         <v>2.7E-2</v>
       </c>
-      <c r="L13" s="44" t="s">
+      <c r="L14" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="M13" s="37" t="s">
+      <c r="M14" s="31" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A14" s="12" t="s">
+    <row r="15" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A15" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F15" s="21">
         <v>1593440</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G15" s="21">
         <v>1</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H15" s="22">
         <v>0.36</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I15" s="22">
         <v>0.32</v>
       </c>
-      <c r="J14" s="3">
-        <f>G14*H14</f>
+      <c r="J15" s="22">
+        <f>G15*H15</f>
         <v>0.36</v>
       </c>
-      <c r="K14" s="3">
-        <f>G14*I14</f>
+      <c r="K15" s="22">
+        <f>G15*I15</f>
         <v>0.32</v>
       </c>
-      <c r="L14" s="36" t="s">
+      <c r="L15" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="M14" s="13" t="s">
+      <c r="M15" s="13" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A15" s="12" t="s">
+    <row r="16" spans="1:31" ht="15.75" customHeight="1">
+      <c r="A16" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="21">
         <v>1882283</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G16" s="21">
         <v>3</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H16" s="22">
         <v>4.88</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I16" s="22">
         <v>3.47</v>
       </c>
-      <c r="J15" s="3">
-        <f>G15*H15</f>
+      <c r="J16" s="22">
+        <f>G16*H16</f>
         <v>14.64</v>
       </c>
-      <c r="K15" s="3">
-        <f>G15*I15</f>
+      <c r="K16" s="22">
+        <f>G16*I16</f>
         <v>10.41</v>
       </c>
-      <c r="L15" s="44" t="s">
+      <c r="L16" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="M15" s="13" t="s">
+      <c r="M16" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A16" s="12" t="s">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A17" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="21">
         <v>1689419</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G17" s="21">
         <v>1</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H17" s="22">
         <v>11.86</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I17" s="22">
         <v>5.83</v>
       </c>
-      <c r="J16" s="3">
-        <f>G16*H16</f>
+      <c r="J17" s="22">
+        <f>G17*H17</f>
         <v>11.86</v>
       </c>
-      <c r="K16" s="3">
-        <f>G16*I16</f>
+      <c r="K17" s="22">
+        <f>G17*I17</f>
         <v>5.83</v>
       </c>
-      <c r="L16" s="44" t="s">
+      <c r="L17" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="M16" s="13" t="s">
+      <c r="M17" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="12" t="s">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A18" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D18" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F18" s="21">
         <v>9306803</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G18" s="21">
         <v>1</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H18" s="22">
         <v>1.7</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I18" s="22">
         <v>1.51</v>
       </c>
-      <c r="J17" s="3">
-        <f>G17*H17</f>
+      <c r="J18" s="22">
+        <f>G18*H18</f>
         <v>1.7</v>
       </c>
-      <c r="K17" s="3">
-        <f>G17*I17</f>
+      <c r="K18" s="22">
+        <f>G18*I18</f>
         <v>1.51</v>
       </c>
-      <c r="L17" s="44" t="s">
+      <c r="L18" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="M17" s="13" t="s">
+      <c r="M18" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="12" t="s">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A19" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B19" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C19" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E19" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="21">
         <v>8529833</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G19" s="21">
         <v>1</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H19" s="22">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I19" s="22">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="J18" s="3">
-        <f>G18*H18</f>
+      <c r="J19" s="22">
+        <f>G19*H19</f>
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="K18" s="3">
-        <f>G18*I18</f>
+      <c r="K19" s="22">
+        <f>G19*I19</f>
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="L18" s="34" t="s">
+      <c r="L19" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="M18" s="33" t="s">
+      <c r="M19" s="14" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="12" t="s">
+    <row r="20" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A20" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="43" t="s">
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2">
+      <c r="F20" s="21"/>
+      <c r="G20" s="21">
         <v>1</v>
       </c>
-      <c r="H19" s="3">
-        <f>17.84/3</f>
-        <v>5.9466666666666663</v>
-      </c>
-      <c r="I19" s="3">
+      <c r="H20" s="22">
+        <f>((17.84/3)/$B$28)*(1-$B$27)</f>
+        <v>3.4586211074760693</v>
+      </c>
+      <c r="I20" s="22">
         <f>Tableau3[[#This Row],[€ / u / 1pc]]/5</f>
-        <v>1.1893333333333334</v>
-      </c>
-      <c r="J19" s="3">
-        <f>G19*H19</f>
-        <v>5.9466666666666663</v>
-      </c>
-      <c r="K19" s="3">
-        <f>G19*I19</f>
-        <v>1.1893333333333334</v>
-      </c>
-      <c r="L19" s="4" t="s">
+        <v>0.69172422149521384</v>
+      </c>
+      <c r="J20" s="22">
+        <f>G20*H20</f>
+        <v>3.4586211074760693</v>
+      </c>
+      <c r="K20" s="22">
+        <f>G20*I20</f>
+        <v>0.69172422149521384</v>
+      </c>
+      <c r="L20" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="M19" s="14"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="12" t="s">
+      <c r="M20" s="38"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A21" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F21" s="21">
         <v>2073537</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G21" s="21">
         <v>16</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H21" s="22">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I21" s="22">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="J20" s="3">
-        <f>G20*H20</f>
-        <v>0.128</v>
-      </c>
-      <c r="K20" s="3">
-        <f>G20*I20</f>
-        <v>0.128</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="M20" s="13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A21" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F21" s="2">
-        <v>2073570</v>
-      </c>
-      <c r="G21" s="2">
-        <v>16</v>
-      </c>
-      <c r="H21" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I21" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="J21" s="3">
+      <c r="J21" s="22">
         <f>G21*H21</f>
         <v>0.128</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="22">
         <f>G21*I21</f>
         <v>0.128</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="L21" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A22" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="21">
+        <v>2073570</v>
+      </c>
+      <c r="G22" s="21">
+        <v>16</v>
+      </c>
+      <c r="H22" s="22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I22" s="22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J22" s="22">
+        <f>G22*H22</f>
+        <v>0.128</v>
+      </c>
+      <c r="K22" s="22">
+        <f>G22*I22</f>
+        <v>0.128</v>
+      </c>
+      <c r="L22" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="M21" s="13" t="s">
+      <c r="M22" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="12" t="s">
+    <row r="23" spans="1:13" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A23" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F23" s="21">
         <v>2073461</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G23" s="21">
         <v>3</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H23" s="22">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I23" s="22">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="J22" s="3">
-        <f>G22*H22</f>
+      <c r="J23" s="22">
+        <f>G23*H23</f>
         <v>2.4E-2</v>
       </c>
-      <c r="K22" s="3">
-        <f>G22*I22</f>
+      <c r="K23" s="22">
+        <f>G23*I23</f>
         <v>2.4E-2</v>
       </c>
-      <c r="L22" s="32" t="s">
+      <c r="L23" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="M22" s="13" t="s">
+      <c r="M23" s="13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="11" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A23" s="12" t="s">
+    <row r="24" spans="1:13" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A24" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F24" s="21">
         <v>2073388</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G24" s="21">
         <v>1</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H24" s="22">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I24" s="22">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="J23" s="3">
-        <f>G23*H23</f>
+      <c r="J24" s="22">
+        <f>G24*H24</f>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="K23" s="3">
-        <f>G23*I23</f>
+      <c r="K24" s="22">
+        <f>G24*I24</f>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="L23" s="30" t="s">
+      <c r="L24" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="M23" s="31" t="s">
+      <c r="M24" s="13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="21" t="s">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A25" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B25" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C25" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D25" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E25" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F25" s="41">
         <v>9238760</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G25" s="41">
         <v>1</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H25" s="42">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I24" s="23">
+      <c r="I25" s="42">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J24" s="24">
-        <f>G24*H24</f>
+      <c r="J25" s="43">
+        <f>G25*H25</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K24" s="24">
-        <f>G24*I24</f>
+      <c r="K25" s="43">
+        <f>G25*I25</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L24" s="25" t="s">
+      <c r="L25" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="M24" s="26" t="s">
+      <c r="M25" s="45" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A26" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6">
-        <f>SUM(G3:G24)</f>
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3">
+        <f>SUM(G4:G25)</f>
         <v>130</v>
       </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="7">
-        <f>SUM(J3:J24)</f>
-        <v>40.884666666666675</v>
-      </c>
-      <c r="K25" s="7">
-        <f>SUM(K3:K24)</f>
-        <v>23.375333333333337</v>
-      </c>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="19">
+        <f>SUM(J4:J25)</f>
+        <v>38.236621107476076</v>
+      </c>
+      <c r="K26" s="19">
+        <f>SUM(K4:K25)</f>
+        <v>22.749724221495217</v>
+      </c>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="A27" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="J27" s="49">
+        <f>J26*B27</f>
+        <v>7.6473242214952153</v>
+      </c>
+      <c r="K27" s="50">
+        <f>K26*B27</f>
+        <v>4.549944844299044</v>
+      </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="A28" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="B28" s="56">
+        <v>1.3754999999999999</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="J28" s="52">
+        <f>J26+J27</f>
+        <v>45.883945328971294</v>
+      </c>
+      <c r="K28" s="53">
+        <f>K26+K27</f>
+        <v>27.299669065794262</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
     </row>
     <row r="33" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
     </row>
     <row r="34" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
     </row>
     <row r="35" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
     </row>
     <row r="36" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
     </row>
     <row r="37" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
     </row>
     <row r="38" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
     </row>
     <row r="39" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
     </row>
     <row r="40" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
     </row>
     <row r="41" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
     </row>
     <row r="42" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
     </row>
     <row r="43" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
     </row>
     <row r="44" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
     </row>
     <row r="45" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
     </row>
     <row r="46" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
     </row>
     <row r="47" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
     </row>
     <row r="48" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
     </row>
     <row r="49" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
     </row>
     <row r="50" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
     </row>
     <row r="51" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
     </row>
     <row r="52" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
     </row>
     <row r="53" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
     </row>
     <row r="54" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
     </row>
     <row r="55" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
     </row>
     <row r="56" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
     </row>
     <row r="57" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
     </row>
     <row r="58" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
     </row>
     <row r="59" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
     </row>
     <row r="60" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
     </row>
     <row r="61" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
     </row>
     <row r="62" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
     </row>
     <row r="63" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
     </row>
     <row r="64" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
     </row>
     <row r="65" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
     </row>
     <row r="66" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
     </row>
     <row r="67" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
     </row>
     <row r="68" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H68" s="8"/>
-      <c r="I68" s="8"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
     </row>
     <row r="69" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
     </row>
     <row r="70" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
     </row>
     <row r="71" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
     </row>
     <row r="72" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
     </row>
     <row r="73" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H73" s="8"/>
-      <c r="I73" s="8"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
     </row>
     <row r="74" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
     </row>
     <row r="75" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
     </row>
     <row r="76" spans="8:9" ht="15.75" customHeight="1">
-      <c r="H76" s="8"/>
-      <c r="I76" s="8"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="8:9" ht="15.75" customHeight="1">
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L3" r:id="rId1"/>
-    <hyperlink ref="M3" r:id="rId2"/>
-    <hyperlink ref="L6" r:id="rId3"/>
-    <hyperlink ref="M6" r:id="rId4"/>
-    <hyperlink ref="L5" r:id="rId5"/>
-    <hyperlink ref="M5" r:id="rId6"/>
-    <hyperlink ref="L4" r:id="rId7"/>
-    <hyperlink ref="M4" r:id="rId8"/>
-    <hyperlink ref="L7" r:id="rId9"/>
-    <hyperlink ref="M7" r:id="rId10"/>
-    <hyperlink ref="L8" r:id="rId11"/>
-    <hyperlink ref="M8" r:id="rId12"/>
-    <hyperlink ref="L9" r:id="rId13"/>
-    <hyperlink ref="M9" r:id="rId14"/>
-    <hyperlink ref="L10" r:id="rId15"/>
-    <hyperlink ref="M10" r:id="rId16"/>
-    <hyperlink ref="L11" r:id="rId17"/>
-    <hyperlink ref="M11" r:id="rId18"/>
-    <hyperlink ref="L12" r:id="rId19"/>
-    <hyperlink ref="M14" r:id="rId20"/>
-    <hyperlink ref="L15" r:id="rId21"/>
-    <hyperlink ref="M15" r:id="rId22"/>
-    <hyperlink ref="L16" r:id="rId23"/>
-    <hyperlink ref="M16" r:id="rId24"/>
-    <hyperlink ref="L17" r:id="rId25"/>
-    <hyperlink ref="M17" r:id="rId26"/>
-    <hyperlink ref="L19" r:id="rId27"/>
-    <hyperlink ref="L20" r:id="rId28"/>
-    <hyperlink ref="M20" r:id="rId29"/>
-    <hyperlink ref="L21" r:id="rId30"/>
-    <hyperlink ref="M21" r:id="rId31"/>
-    <hyperlink ref="L22" r:id="rId32"/>
-    <hyperlink ref="M22" r:id="rId33"/>
-    <hyperlink ref="L24" r:id="rId34"/>
-    <hyperlink ref="M24" r:id="rId35"/>
-    <hyperlink ref="L14" r:id="rId36"/>
-    <hyperlink ref="M13" r:id="rId37"/>
+    <hyperlink ref="L4" r:id="rId1"/>
+    <hyperlink ref="M4" r:id="rId2"/>
+    <hyperlink ref="L7" r:id="rId3"/>
+    <hyperlink ref="M7" r:id="rId4"/>
+    <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="M6" r:id="rId6"/>
+    <hyperlink ref="L5" r:id="rId7"/>
+    <hyperlink ref="M5" r:id="rId8"/>
+    <hyperlink ref="L8" r:id="rId9"/>
+    <hyperlink ref="M8" r:id="rId10"/>
+    <hyperlink ref="L9" r:id="rId11"/>
+    <hyperlink ref="M9" r:id="rId12"/>
+    <hyperlink ref="L10" r:id="rId13"/>
+    <hyperlink ref="M10" r:id="rId14"/>
+    <hyperlink ref="L11" r:id="rId15"/>
+    <hyperlink ref="M11" r:id="rId16"/>
+    <hyperlink ref="L12" r:id="rId17"/>
+    <hyperlink ref="M12" r:id="rId18"/>
+    <hyperlink ref="L13" r:id="rId19"/>
+    <hyperlink ref="M15" r:id="rId20"/>
+    <hyperlink ref="L16" r:id="rId21"/>
+    <hyperlink ref="M16" r:id="rId22"/>
+    <hyperlink ref="L17" r:id="rId23"/>
+    <hyperlink ref="M17" r:id="rId24"/>
+    <hyperlink ref="L18" r:id="rId25"/>
+    <hyperlink ref="M18" r:id="rId26"/>
+    <hyperlink ref="L20" r:id="rId27"/>
+    <hyperlink ref="L21" r:id="rId28"/>
+    <hyperlink ref="M21" r:id="rId29"/>
+    <hyperlink ref="L22" r:id="rId30"/>
+    <hyperlink ref="M22" r:id="rId31"/>
+    <hyperlink ref="L23" r:id="rId32"/>
+    <hyperlink ref="M23" r:id="rId33"/>
+    <hyperlink ref="L25" r:id="rId34"/>
+    <hyperlink ref="M25" r:id="rId35"/>
+    <hyperlink ref="L15" r:id="rId36"/>
+    <hyperlink ref="M14" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
@@ -3705,10 +3424,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="6" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed incorrect capacitor reference in BOM
</commit_message>
<xml_diff>
--- a/hardware/eagle/bom.xlsx
+++ b/hardware/eagle/bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="164">
   <si>
     <t>category</t>
   </si>
@@ -150,18 +150,9 @@
     <t>MULTICOMP</t>
   </si>
   <si>
-    <t>MCCA000153</t>
-  </si>
-  <si>
     <t>Farnell</t>
   </si>
   <si>
-    <t>http://fr.farnell.com/multicomp/mcca000153/condensateur-mlcc-0603-x7r-16v/dp/1759009</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/1723208.pdf</t>
-  </si>
-  <si>
     <t>capacitor</t>
   </si>
   <si>
@@ -514,6 +505,12 @@
   </si>
   <si>
     <t>for the pcb (order in $)</t>
+  </si>
+  <si>
+    <t>http://fr.farnell.com/multicomp/mc0603b332j500ct/condensateur-mlcc-3-3nf-50v-x7r/dp/2320807</t>
+  </si>
+  <si>
+    <t>MC0603B332J500CT</t>
   </si>
 </sst>
 </file>
@@ -523,7 +520,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000;\(#,##0.000\)"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1]"/>
-    <numFmt numFmtId="176" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1110,10 +1107,6 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="23" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1126,7 +1119,11 @@
     <xf numFmtId="165" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="25" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="25" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="25" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1137,30 +1134,6 @@
     <cellStyle name="Pourcentage" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1664,22 +1637,46 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -1725,29 +1722,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A3:M25" headerRowDxfId="17" dataDxfId="0" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A3:M25" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A3:M25"/>
   <sortState ref="A3:M24">
     <sortCondition ref="A2:A24"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="category" totalsRowLabel="Total" dataDxfId="13"/>
-    <tableColumn id="2" name="value/description" dataDxfId="12"/>
-    <tableColumn id="3" name="manufacturer name" dataDxfId="11"/>
-    <tableColumn id="4" name="manufacturer ref" dataDxfId="10"/>
-    <tableColumn id="5" name="vendor name" dataDxfId="9"/>
-    <tableColumn id="6" name="vendor ref" dataDxfId="8"/>
-    <tableColumn id="7" name="qty" dataDxfId="7"/>
-    <tableColumn id="8" name="€ / u / 1pc" dataDxfId="6"/>
-    <tableColumn id="9" name="€ / u / 100pcs" dataDxfId="5"/>
-    <tableColumn id="10" name="€ / 1pc" dataDxfId="4">
+    <tableColumn id="1" name="category" totalsRowLabel="Total" dataDxfId="12"/>
+    <tableColumn id="2" name="value/description" dataDxfId="11"/>
+    <tableColumn id="3" name="manufacturer name" dataDxfId="10"/>
+    <tableColumn id="4" name="manufacturer ref" dataDxfId="9"/>
+    <tableColumn id="5" name="vendor name" dataDxfId="8"/>
+    <tableColumn id="6" name="vendor ref" dataDxfId="7"/>
+    <tableColumn id="7" name="qty" dataDxfId="6"/>
+    <tableColumn id="8" name="€ / u / 1pc" dataDxfId="5"/>
+    <tableColumn id="9" name="€ / u / 100pcs" dataDxfId="4"/>
+    <tableColumn id="10" name="€ / 1pc" dataDxfId="3">
       <calculatedColumnFormula>G4*H4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="€ / 100pc" dataDxfId="3">
+    <tableColumn id="11" name="€ / 100pc" dataDxfId="2">
       <calculatedColumnFormula>G4*I4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="link" dataDxfId="2"/>
-    <tableColumn id="13" name="datasheet" totalsRowFunction="count" dataDxfId="1"/>
+    <tableColumn id="12" name="link" dataDxfId="1"/>
+    <tableColumn id="13" name="datasheet" totalsRowFunction="count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2040,9 +2037,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2063,23 +2060,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18">
-      <c r="A1" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
+      <c r="A1" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
     </row>
     <row r="2" spans="1:31" s="16" customFormat="1" ht="18.75">
       <c r="A2" s="57" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B2" s="57"/>
       <c r="C2" s="57"/>
@@ -2182,11 +2179,11 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="J4" s="22">
-        <f>G4*H4</f>
+        <f t="shared" ref="J4:J25" si="0">G4*H4</f>
         <v>2.8699999999999997</v>
       </c>
       <c r="K4" s="22">
-        <f>G4*I4</f>
+        <f t="shared" ref="K4:K25" si="1">G4*I4</f>
         <v>1.036</v>
       </c>
       <c r="L4" s="23" t="s">
@@ -2225,11 +2222,11 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="J5" s="22">
-        <f>G5*H5</f>
+        <f t="shared" si="0"/>
         <v>1.008</v>
       </c>
       <c r="K5" s="22">
-        <f>G5*I5</f>
+        <f t="shared" si="1"/>
         <v>1.008</v>
       </c>
       <c r="L5" s="23" t="s">
@@ -2268,15 +2265,15 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="J6" s="22">
-        <f>G6*H6</f>
+        <f t="shared" si="0"/>
         <v>0.10799999999999998</v>
       </c>
       <c r="K6" s="22">
-        <f>G6*I6</f>
+        <f t="shared" si="1"/>
         <v>0.10799999999999998</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M6" s="13" t="s">
         <v>32</v>
@@ -2311,11 +2308,11 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="J7" s="22">
-        <f>G7*H7</f>
+        <f t="shared" si="0"/>
         <v>0.112</v>
       </c>
       <c r="K7" s="22">
-        <f>G7*I7</f>
+        <f t="shared" si="1"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="L7" s="23" t="s">
@@ -2336,53 +2333,53 @@
         <v>42</v>
       </c>
       <c r="D8" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>44</v>
-      </c>
       <c r="F8" s="21">
-        <v>1759009</v>
+        <v>2320807</v>
       </c>
       <c r="G8" s="21">
         <v>8</v>
       </c>
-      <c r="H8" s="22">
-        <v>8.9999999999999993E-3</v>
+      <c r="H8" s="28">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="I8" s="22">
-        <v>8.9999999999999993E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="J8" s="22">
-        <f>G8*H8</f>
-        <v>7.1999999999999995E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="K8" s="22">
-        <f>G8*I8</f>
-        <v>7.1999999999999995E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1">
       <c r="A9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="E9" s="21" t="s">
         <v>48</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>51</v>
       </c>
       <c r="F9" s="21">
         <v>1759027</v>
@@ -2397,35 +2394,35 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J9" s="22">
-        <f>G9*H9</f>
+        <f t="shared" si="0"/>
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="K9" s="22">
-        <f>G9*I9</f>
+        <f t="shared" si="1"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="15.75" customHeight="1">
       <c r="A10" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>55</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>58</v>
       </c>
       <c r="F10" s="21">
         <v>2320806</v>
@@ -2440,35 +2437,35 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J10" s="22">
-        <f>G10*H10</f>
+        <f t="shared" si="0"/>
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="K10" s="22">
-        <f>G10*I10</f>
+        <f t="shared" si="1"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:31" s="16" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="E11" s="21" t="s">
         <v>62</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>65</v>
       </c>
       <c r="F11" s="21">
         <v>1759037</v>
@@ -2483,35 +2480,35 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="J11" s="22">
-        <f>G11*H11</f>
+        <f t="shared" si="0"/>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K11" s="22">
-        <f>G11*I11</f>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:31" s="11" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="E12" s="21" t="s">
         <v>69</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>72</v>
       </c>
       <c r="F12" s="26">
         <v>1593445</v>
@@ -2526,38 +2523,38 @@
         <v>0.64</v>
       </c>
       <c r="J12" s="22">
-        <f>G12*H12</f>
+        <f t="shared" si="0"/>
         <v>0.83</v>
       </c>
       <c r="K12" s="22">
-        <f>G12*I12</f>
+        <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1">
       <c r="A13" s="20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G13" s="21">
         <v>2</v>
@@ -2571,30 +2568,30 @@
         <v>0.25600000000000001</v>
       </c>
       <c r="J13" s="22">
-        <f>G13*H13</f>
+        <f t="shared" si="0"/>
         <v>0.64000000000000012</v>
       </c>
       <c r="K13" s="22">
-        <f>G13*I13</f>
+        <f t="shared" si="1"/>
         <v>0.51200000000000001</v>
       </c>
       <c r="L13" s="29" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M13" s="13"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1">
       <c r="A14" s="20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>17</v>
@@ -2612,35 +2609,35 @@
         <v>2.7E-2</v>
       </c>
       <c r="J14" s="22">
-        <f>G14*H14</f>
+        <f t="shared" si="0"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="K14" s="22">
-        <f>G14*I14</f>
+        <f t="shared" si="1"/>
         <v>2.7E-2</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M14" s="31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1">
       <c r="A15" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="E15" s="21" t="s">
         <v>79</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>82</v>
       </c>
       <c r="F15" s="21">
         <v>1593440</v>
@@ -2655,35 +2652,35 @@
         <v>0.32</v>
       </c>
       <c r="J15" s="22">
-        <f>G15*H15</f>
+        <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
       <c r="K15" s="22">
-        <f>G15*I15</f>
+        <f t="shared" si="1"/>
         <v>0.32</v>
       </c>
       <c r="L15" s="32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1">
       <c r="A16" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="E16" s="21" t="s">
         <v>86</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>89</v>
       </c>
       <c r="F16" s="21">
         <v>1882283</v>
@@ -2698,35 +2695,35 @@
         <v>3.47</v>
       </c>
       <c r="J16" s="22">
-        <f>G16*H16</f>
+        <f t="shared" si="0"/>
         <v>14.64</v>
       </c>
       <c r="K16" s="22">
-        <f>G16*I16</f>
+        <f t="shared" si="1"/>
         <v>10.41</v>
       </c>
       <c r="L16" s="29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M16" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="E17" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>96</v>
       </c>
       <c r="F17" s="21">
         <v>1689419</v>
@@ -2741,35 +2738,35 @@
         <v>5.83</v>
       </c>
       <c r="J17" s="22">
-        <f>G17*H17</f>
+        <f t="shared" si="0"/>
         <v>11.86</v>
       </c>
       <c r="K17" s="22">
-        <f>G17*I17</f>
+        <f t="shared" si="1"/>
         <v>5.83</v>
       </c>
       <c r="L17" s="29" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="E18" s="21" t="s">
         <v>100</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>103</v>
       </c>
       <c r="F18" s="21">
         <v>9306803</v>
@@ -2784,32 +2781,32 @@
         <v>1.51</v>
       </c>
       <c r="J18" s="22">
-        <f>G18*H18</f>
+        <f t="shared" si="0"/>
         <v>1.7</v>
       </c>
       <c r="K18" s="22">
-        <f>G18*I18</f>
+        <f t="shared" si="1"/>
         <v>1.51</v>
       </c>
       <c r="L18" s="29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M18" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>143</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>146</v>
       </c>
       <c r="E19" s="35" t="s">
         <v>17</v>
@@ -2827,29 +2824,29 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="J19" s="22">
-        <f>G19*H19</f>
+        <f t="shared" si="0"/>
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="K19" s="22">
-        <f>G19*I19</f>
+        <f t="shared" si="1"/>
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M19" s="14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B20" s="36"/>
       <c r="C20" s="36"/>
       <c r="D20" s="21"/>
       <c r="E20" s="37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="21">
@@ -2864,33 +2861,33 @@
         <v>0.69172422149521384</v>
       </c>
       <c r="J20" s="22">
-        <f>G20*H20</f>
+        <f t="shared" si="0"/>
         <v>3.4586211074760693</v>
       </c>
       <c r="K20" s="22">
-        <f>G20*I20</f>
+        <f t="shared" si="1"/>
         <v>0.69172422149521384</v>
       </c>
       <c r="L20" s="23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M20" s="38"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="E21" s="21" t="s">
         <v>110</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>113</v>
       </c>
       <c r="F21" s="21">
         <v>2073537</v>
@@ -2905,35 +2902,35 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J21" s="22">
-        <f>G21*H21</f>
+        <f t="shared" si="0"/>
         <v>0.128</v>
       </c>
       <c r="K21" s="22">
-        <f>G21*I21</f>
+        <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
       <c r="L21" s="23" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="E22" s="21" t="s">
         <v>117</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>120</v>
       </c>
       <c r="F22" s="21">
         <v>2073570</v>
@@ -2948,35 +2945,35 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J22" s="22">
-        <f>G22*H22</f>
+        <f t="shared" si="0"/>
         <v>0.128</v>
       </c>
       <c r="K22" s="22">
-        <f>G22*I22</f>
+        <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
       <c r="L22" s="23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="E23" s="21" t="s">
         <v>124</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>127</v>
       </c>
       <c r="F23" s="21">
         <v>2073461</v>
@@ -2991,32 +2988,32 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J23" s="22">
-        <f>G23*H23</f>
+        <f t="shared" si="0"/>
         <v>2.4E-2</v>
       </c>
       <c r="K23" s="22">
-        <f>G23*I23</f>
+        <f t="shared" si="1"/>
         <v>2.4E-2</v>
       </c>
       <c r="L23" s="39" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="M23" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>17</v>
@@ -3034,35 +3031,35 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="J24" s="22">
-        <f>G24*H24</f>
+        <f t="shared" si="0"/>
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="K24" s="22">
-        <f>G24*I24</f>
+        <f t="shared" si="1"/>
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M24" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="E25" s="41" t="s">
         <v>131</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="D25" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="41" t="s">
-        <v>134</v>
       </c>
       <c r="F25" s="41">
         <v>9238760</v>
@@ -3077,23 +3074,23 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J25" s="43">
-        <f>G25*H25</f>
+        <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="K25" s="43">
-        <f>G25*I25</f>
+        <f t="shared" si="1"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="L25" s="44" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M25" s="45" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
@@ -3108,59 +3105,59 @@
       <c r="I26" s="18"/>
       <c r="J26" s="19">
         <f>SUM(J4:J25)</f>
-        <v>38.236621107476076</v>
+        <v>38.22862110747608</v>
       </c>
       <c r="K26" s="19">
         <f>SUM(K4:K25)</f>
-        <v>22.749724221495217</v>
+        <v>22.733724221495216</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" s="53">
+        <v>0.2</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="B27" s="55">
-        <v>0.2</v>
-      </c>
-      <c r="C27" s="54" t="s">
-        <v>163</v>
-      </c>
-      <c r="H27" s="4"/>
-      <c r="I27" s="48" t="s">
+      <c r="J27" s="47">
+        <f>J26*B27</f>
+        <v>7.6457242214952164</v>
+      </c>
+      <c r="K27" s="48">
+        <f>K26*B27</f>
+        <v>4.5467448442990435</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A28" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="54">
+        <v>1.3754999999999999</v>
+      </c>
+      <c r="C28" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="J27" s="49">
-        <f>J26*B27</f>
-        <v>7.6473242214952153</v>
-      </c>
-      <c r="K27" s="50">
-        <f>K26*B27</f>
-        <v>4.549944844299044</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="54" t="s">
+      <c r="H28" s="4"/>
+      <c r="I28" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="B28" s="56">
-        <v>1.3754999999999999</v>
-      </c>
-      <c r="C28" s="54" t="s">
-        <v>164</v>
-      </c>
-      <c r="H28" s="4"/>
-      <c r="I28" s="51" t="s">
-        <v>162</v>
-      </c>
-      <c r="J28" s="52">
+      <c r="J28" s="50">
         <f>J26+J27</f>
-        <v>45.883945328971294</v>
-      </c>
-      <c r="K28" s="53">
+        <v>45.874345328971295</v>
+      </c>
+      <c r="K28" s="51">
         <f>K26+K27</f>
-        <v>27.299669065794262</v>
+        <v>27.280469065794257</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
@@ -3373,40 +3370,38 @@
     <hyperlink ref="M6" r:id="rId6"/>
     <hyperlink ref="L5" r:id="rId7"/>
     <hyperlink ref="M5" r:id="rId8"/>
-    <hyperlink ref="L8" r:id="rId9"/>
-    <hyperlink ref="M8" r:id="rId10"/>
-    <hyperlink ref="L9" r:id="rId11"/>
-    <hyperlink ref="M9" r:id="rId12"/>
-    <hyperlink ref="L10" r:id="rId13"/>
-    <hyperlink ref="M10" r:id="rId14"/>
-    <hyperlink ref="L11" r:id="rId15"/>
-    <hyperlink ref="M11" r:id="rId16"/>
-    <hyperlink ref="L12" r:id="rId17"/>
-    <hyperlink ref="M12" r:id="rId18"/>
-    <hyperlink ref="L13" r:id="rId19"/>
-    <hyperlink ref="M15" r:id="rId20"/>
-    <hyperlink ref="L16" r:id="rId21"/>
-    <hyperlink ref="M16" r:id="rId22"/>
-    <hyperlink ref="L17" r:id="rId23"/>
-    <hyperlink ref="M17" r:id="rId24"/>
-    <hyperlink ref="L18" r:id="rId25"/>
-    <hyperlink ref="M18" r:id="rId26"/>
-    <hyperlink ref="L20" r:id="rId27"/>
-    <hyperlink ref="L21" r:id="rId28"/>
-    <hyperlink ref="M21" r:id="rId29"/>
-    <hyperlink ref="L22" r:id="rId30"/>
-    <hyperlink ref="M22" r:id="rId31"/>
-    <hyperlink ref="L23" r:id="rId32"/>
-    <hyperlink ref="M23" r:id="rId33"/>
-    <hyperlink ref="L25" r:id="rId34"/>
-    <hyperlink ref="M25" r:id="rId35"/>
-    <hyperlink ref="L15" r:id="rId36"/>
-    <hyperlink ref="M14" r:id="rId37"/>
+    <hyperlink ref="L9" r:id="rId9"/>
+    <hyperlink ref="M9" r:id="rId10"/>
+    <hyperlink ref="L10" r:id="rId11"/>
+    <hyperlink ref="M10" r:id="rId12"/>
+    <hyperlink ref="L11" r:id="rId13"/>
+    <hyperlink ref="M11" r:id="rId14"/>
+    <hyperlink ref="L12" r:id="rId15"/>
+    <hyperlink ref="M12" r:id="rId16"/>
+    <hyperlink ref="L13" r:id="rId17"/>
+    <hyperlink ref="M15" r:id="rId18"/>
+    <hyperlink ref="L16" r:id="rId19"/>
+    <hyperlink ref="M16" r:id="rId20"/>
+    <hyperlink ref="L17" r:id="rId21"/>
+    <hyperlink ref="M17" r:id="rId22"/>
+    <hyperlink ref="L18" r:id="rId23"/>
+    <hyperlink ref="M18" r:id="rId24"/>
+    <hyperlink ref="L20" r:id="rId25"/>
+    <hyperlink ref="L21" r:id="rId26"/>
+    <hyperlink ref="M21" r:id="rId27"/>
+    <hyperlink ref="L22" r:id="rId28"/>
+    <hyperlink ref="M22" r:id="rId29"/>
+    <hyperlink ref="L23" r:id="rId30"/>
+    <hyperlink ref="M23" r:id="rId31"/>
+    <hyperlink ref="L25" r:id="rId32"/>
+    <hyperlink ref="M25" r:id="rId33"/>
+    <hyperlink ref="L15" r:id="rId34"/>
+    <hyperlink ref="M14" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
   <tableParts count="1">
-    <tablePart r:id="rId39"/>
+    <tablePart r:id="rId37"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3425,10 +3420,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected BOM pcb price
</commit_message>
<xml_diff>
--- a/hardware/eagle/bom.xlsx
+++ b/hardware/eagle/bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="162">
   <si>
     <t>category</t>
   </si>
@@ -489,9 +489,6 @@
     <t>taxe rate =</t>
   </si>
   <si>
-    <t>1 € =</t>
-  </si>
-  <si>
     <t>taxes excluded</t>
   </si>
   <si>
@@ -502,9 +499,6 @@
   </si>
   <si>
     <t>France VAT</t>
-  </si>
-  <si>
-    <t>for the pcb (order in $)</t>
   </si>
   <si>
     <t>http://fr.farnell.com/multicomp/mc0603b332j500ct/condensateur-mlcc-3-3nf-50v-x7r/dp/2320807</t>
@@ -1058,7 +1052,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1119,7 +1113,6 @@
     <xf numFmtId="165" fontId="0" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="25" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="25" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1127,6 +1120,8 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2037,9 +2032,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2060,34 +2055,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="2" spans="1:31" s="16" customFormat="1" ht="18.75">
-      <c r="A2" s="57" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
+      <c r="A2" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
     </row>
@@ -2333,7 +2328,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>43</v>
@@ -2359,7 +2354,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M8" s="13" t="s">
         <v>26</v>
@@ -2853,20 +2848,20 @@
         <v>1</v>
       </c>
       <c r="H20" s="22">
-        <f>((17.84/3)/$B$28)*(1-$B$27)</f>
-        <v>3.4586211074760693</v>
+        <f>(18.56/3)*(1-$B$27)</f>
+        <v>4.9493333333333336</v>
       </c>
       <c r="I20" s="22">
         <f>Tableau3[[#This Row],[€ / u / 1pc]]/5</f>
-        <v>0.69172422149521384</v>
+        <v>0.98986666666666667</v>
       </c>
       <c r="J20" s="22">
         <f t="shared" si="0"/>
-        <v>3.4586211074760693</v>
+        <v>4.9493333333333336</v>
       </c>
       <c r="K20" s="22">
         <f t="shared" si="1"/>
-        <v>0.69172422149521384</v>
+        <v>0.98986666666666667</v>
       </c>
       <c r="L20" s="23" t="s">
         <v>105</v>
@@ -3105,11 +3100,11 @@
       <c r="I26" s="18"/>
       <c r="J26" s="19">
         <f>SUM(J4:J25)</f>
-        <v>38.22862110747608</v>
+        <v>39.719333333333346</v>
       </c>
       <c r="K26" s="19">
         <f>SUM(K4:K25)</f>
-        <v>22.733724221495216</v>
+        <v>23.031866666666669</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -3122,42 +3117,36 @@
         <v>0.2</v>
       </c>
       <c r="C27" s="52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J27" s="47">
         <f>J26*B27</f>
-        <v>7.6457242214952164</v>
+        <v>7.9438666666666693</v>
       </c>
       <c r="K27" s="48">
         <f>K26*B27</f>
-        <v>4.5467448442990435</v>
+        <v>4.6063733333333339</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="B28" s="54">
-        <v>1.3754999999999999</v>
-      </c>
-      <c r="C28" s="52" t="s">
-        <v>161</v>
-      </c>
+      <c r="A28" s="57"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="57"/>
       <c r="H28" s="4"/>
       <c r="I28" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J28" s="50">
         <f>J26+J27</f>
-        <v>45.874345328971295</v>
+        <v>47.663200000000018</v>
       </c>
       <c r="K28" s="51">
         <f>K26+K27</f>
-        <v>27.280469065794257</v>
+        <v>27.638240000000003</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Updated BOM and Farnell basket
</commit_message>
<xml_diff>
--- a/hardware/eagle/bom.xlsx
+++ b/hardware/eagle/bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="172">
   <si>
     <t>category</t>
   </si>
@@ -505,6 +505,36 @@
   </si>
   <si>
     <t>MC0603B332J500CT</t>
+  </si>
+  <si>
+    <t>http://www.dx.com/p/audio-4-female-jack-rca-socket-connectors-10-piece-pack-138307</t>
+  </si>
+  <si>
+    <t>Audio 4 Female Jack RCA Socket Connectors (10-Piece Pack)</t>
+  </si>
+  <si>
+    <t>http://www.dx.com/p/dual-sockets-3-5mm-av-jack-connectors-red-black-silver-10-pack-122545</t>
+  </si>
+  <si>
+    <t>Replacement Audio RCA Chassis Connectors - Red + Black + Silver (10-Pack)</t>
+  </si>
+  <si>
+    <t>http://www.dx.com/p/double-side-qfp-qfn-tqfp-lqfp-16-80-pin-to-dip-adapter-breakout-board-module-for-arduino-206458</t>
+  </si>
+  <si>
+    <t>Double-Side QFP / QFN / TQFP / LQFP 16-80-pin to DIP Adapter</t>
+  </si>
+  <si>
+    <t>http://www.dx.com/p/jtron-aluminum-pcb-receiver-shell-junction-box-black-290724</t>
+  </si>
+  <si>
+    <t>Jtron Aluminum PCB / Receiver Shell / Junction Box - Black</t>
+  </si>
+  <si>
+    <t>Dual-Channel Audio RCA Socket (5 PCS)</t>
+  </si>
+  <si>
+    <t>http://www.dx.com/p/dual-channel-audio-rca-socket-5-pcs-303101</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1082,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1083,7 +1113,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1122,6 +1151,8 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1719,8 +1750,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A3:M25" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A3:M25"/>
-  <sortState ref="A3:M24">
-    <sortCondition ref="A2:A24"/>
+  <sortState ref="A4:M25">
+    <sortCondition ref="A3:A25"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" name="category" totalsRowLabel="Total" dataDxfId="12"/>
@@ -2033,8 +2064,8 @@
   <dimension ref="A1:AE77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2055,34 +2086,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:31" s="16" customFormat="1" ht="18.75">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
     </row>
@@ -2174,11 +2205,11 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="J4" s="22">
-        <f t="shared" ref="J4:J25" si="0">G4*H4</f>
+        <f>G4*H4</f>
         <v>2.8699999999999997</v>
       </c>
       <c r="K4" s="22">
-        <f t="shared" ref="K4:K25" si="1">G4*I4</f>
+        <f>G4*I4</f>
         <v>1.036</v>
       </c>
       <c r="L4" s="23" t="s">
@@ -2217,11 +2248,11 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="J5" s="22">
-        <f t="shared" si="0"/>
+        <f>G5*H5</f>
         <v>1.008</v>
       </c>
       <c r="K5" s="22">
-        <f t="shared" si="1"/>
+        <f>G5*I5</f>
         <v>1.008</v>
       </c>
       <c r="L5" s="23" t="s">
@@ -2260,11 +2291,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="J6" s="22">
-        <f t="shared" si="0"/>
+        <f>G6*H6</f>
         <v>0.10799999999999998</v>
       </c>
       <c r="K6" s="22">
-        <f t="shared" si="1"/>
+        <f>G6*I6</f>
         <v>0.10799999999999998</v>
       </c>
       <c r="L6" s="24" t="s">
@@ -2303,11 +2334,11 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="J7" s="22">
-        <f t="shared" si="0"/>
+        <f>G7*H7</f>
         <v>0.112</v>
       </c>
       <c r="K7" s="22">
-        <f t="shared" si="1"/>
+        <f>G7*I7</f>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="L7" s="23" t="s">
@@ -2346,11 +2377,11 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="J8" s="22">
-        <f t="shared" si="0"/>
+        <f>G8*H8</f>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="K8" s="22">
-        <f t="shared" si="1"/>
+        <f>G8*I8</f>
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="L8" s="23" t="s">
@@ -2389,11 +2420,11 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J9" s="22">
-        <f t="shared" si="0"/>
+        <f>G9*H9</f>
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="K9" s="22">
-        <f t="shared" si="1"/>
+        <f>G9*I9</f>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="L9" s="23" t="s">
@@ -2432,11 +2463,11 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J10" s="22">
-        <f t="shared" si="0"/>
+        <f>G10*H10</f>
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="K10" s="22">
-        <f t="shared" si="1"/>
+        <f>G10*I10</f>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="L10" s="23" t="s">
@@ -2475,11 +2506,11 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="J11" s="22">
-        <f t="shared" si="0"/>
+        <f>G11*H11</f>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K11" s="22">
-        <f t="shared" si="1"/>
+        <f>G11*I11</f>
         <v>0.03</v>
       </c>
       <c r="L11" s="23" t="s">
@@ -2518,11 +2549,11 @@
         <v>0.64</v>
       </c>
       <c r="J12" s="22">
-        <f t="shared" si="0"/>
+        <f>G12*H12</f>
         <v>0.83</v>
       </c>
       <c r="K12" s="22">
-        <f t="shared" si="1"/>
+        <f>G12*I12</f>
         <v>0.64</v>
       </c>
       <c r="L12" s="27" t="s">
@@ -2563,11 +2594,11 @@
         <v>0.25600000000000001</v>
       </c>
       <c r="J13" s="22">
-        <f t="shared" si="0"/>
+        <f>G13*H13</f>
         <v>0.64000000000000012</v>
       </c>
       <c r="K13" s="22">
-        <f t="shared" si="1"/>
+        <f>G13*I13</f>
         <v>0.51200000000000001</v>
       </c>
       <c r="L13" s="29" t="s">
@@ -2577,88 +2608,88 @@
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1">
       <c r="A14" s="20" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>17</v>
+        <v>76</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>79</v>
       </c>
       <c r="F14" s="26">
-        <v>1593411</v>
+        <v>1593440</v>
       </c>
       <c r="G14" s="21">
         <v>1</v>
       </c>
       <c r="H14" s="22">
-        <v>6.5000000000000002E-2</v>
+        <v>0.36</v>
       </c>
       <c r="I14" s="22">
-        <v>2.7E-2</v>
+        <v>0.32</v>
       </c>
       <c r="J14" s="22">
-        <f t="shared" si="0"/>
-        <v>6.5000000000000002E-2</v>
+        <f>G14*H14</f>
+        <v>0.36</v>
       </c>
       <c r="K14" s="22">
-        <f t="shared" si="1"/>
-        <v>2.7E-2</v>
-      </c>
-      <c r="L14" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="M14" s="31" t="s">
-        <v>150</v>
+        <f>G14*I14</f>
+        <v>0.32</v>
+      </c>
+      <c r="L14" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1">
       <c r="A15" s="20" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>79</v>
+        <v>147</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" s="58" t="s">
+        <v>17</v>
       </c>
       <c r="F15" s="21">
-        <v>1593440</v>
+        <v>1593411</v>
       </c>
       <c r="G15" s="21">
         <v>1</v>
       </c>
       <c r="H15" s="22">
-        <v>0.36</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="I15" s="22">
-        <v>0.32</v>
+        <v>2.7E-2</v>
       </c>
       <c r="J15" s="22">
-        <f t="shared" si="0"/>
-        <v>0.36</v>
+        <f>G15*H15</f>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="K15" s="22">
-        <f t="shared" si="1"/>
-        <v>0.32</v>
-      </c>
-      <c r="L15" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="M15" s="13" t="s">
-        <v>81</v>
+        <f>G15*I15</f>
+        <v>2.7E-2</v>
+      </c>
+      <c r="L15" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="M15" s="30" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1">
@@ -2690,11 +2721,11 @@
         <v>3.47</v>
       </c>
       <c r="J16" s="22">
-        <f t="shared" si="0"/>
+        <f>G16*H16</f>
         <v>14.64</v>
       </c>
       <c r="K16" s="22">
-        <f t="shared" si="1"/>
+        <f>G16*I16</f>
         <v>10.41</v>
       </c>
       <c r="L16" s="29" t="s">
@@ -2733,11 +2764,11 @@
         <v>5.83</v>
       </c>
       <c r="J17" s="22">
-        <f t="shared" si="0"/>
+        <f>G17*H17</f>
         <v>11.86</v>
       </c>
       <c r="K17" s="22">
-        <f t="shared" si="1"/>
+        <f>G17*I17</f>
         <v>5.83</v>
       </c>
       <c r="L17" s="29" t="s">
@@ -2757,7 +2788,7 @@
       <c r="C18" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="32" t="s">
         <v>99</v>
       </c>
       <c r="E18" s="21" t="s">
@@ -2776,11 +2807,11 @@
         <v>1.51</v>
       </c>
       <c r="J18" s="22">
-        <f t="shared" si="0"/>
+        <f>G18*H18</f>
         <v>1.7</v>
       </c>
       <c r="K18" s="22">
-        <f t="shared" si="1"/>
+        <f>G18*I18</f>
         <v>1.51</v>
       </c>
       <c r="L18" s="29" t="s">
@@ -2794,16 +2825,16 @@
       <c r="A19" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="33" t="s">
         <v>142</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="34" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="21">
@@ -2819,11 +2850,11 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="J19" s="22">
-        <f t="shared" si="0"/>
+        <f>G19*H19</f>
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="K19" s="22">
-        <f t="shared" si="1"/>
+        <f>G19*I19</f>
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="L19" s="15" t="s">
@@ -2837,10 +2868,10 @@
       <c r="A20" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="36" t="s">
         <v>104</v>
       </c>
       <c r="F20" s="21"/>
@@ -2856,17 +2887,17 @@
         <v>0.98986666666666667</v>
       </c>
       <c r="J20" s="22">
-        <f t="shared" si="0"/>
+        <f>G20*H20</f>
         <v>4.9493333333333336</v>
       </c>
       <c r="K20" s="22">
-        <f t="shared" si="1"/>
+        <f>G20*I20</f>
         <v>0.98986666666666667</v>
       </c>
       <c r="L20" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="M20" s="38"/>
+      <c r="M20" s="37"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="20" t="s">
@@ -2897,11 +2928,11 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J21" s="22">
-        <f t="shared" si="0"/>
+        <f>G21*H21</f>
         <v>0.128</v>
       </c>
       <c r="K21" s="22">
-        <f t="shared" si="1"/>
+        <f>G21*I21</f>
         <v>0.128</v>
       </c>
       <c r="L21" s="23" t="s">
@@ -2940,11 +2971,11 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J22" s="22">
-        <f t="shared" si="0"/>
+        <f>G22*H22</f>
         <v>0.128</v>
       </c>
       <c r="K22" s="22">
-        <f t="shared" si="1"/>
+        <f>G22*I22</f>
         <v>0.128</v>
       </c>
       <c r="L22" s="23" t="s">
@@ -2983,14 +3014,14 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J23" s="22">
-        <f t="shared" si="0"/>
+        <f>G23*H23</f>
         <v>2.4E-2</v>
       </c>
       <c r="K23" s="22">
-        <f t="shared" si="1"/>
+        <f>G23*I23</f>
         <v>2.4E-2</v>
       </c>
-      <c r="L23" s="39" t="s">
+      <c r="L23" s="38" t="s">
         <v>125</v>
       </c>
       <c r="M23" s="13" t="s">
@@ -3026,11 +3057,11 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="J24" s="22">
-        <f t="shared" si="0"/>
+        <f>G24*H24</f>
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="K24" s="22">
-        <f t="shared" si="1"/>
+        <f>G24*I24</f>
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="L24" s="12" t="s">
@@ -3041,45 +3072,45 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D25" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E25" s="41" t="s">
+      <c r="E25" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="F25" s="41">
+      <c r="F25" s="40">
         <v>9238760</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G25" s="40">
         <v>1</v>
       </c>
-      <c r="H25" s="42">
+      <c r="H25" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I25" s="42">
+      <c r="I25" s="41">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J25" s="43">
-        <f t="shared" si="0"/>
+      <c r="J25" s="42">
+        <f>G25*H25</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K25" s="43">
-        <f t="shared" si="1"/>
+      <c r="K25" s="42">
+        <f>G25*I25</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L25" s="44" t="s">
+      <c r="L25" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="M25" s="45" t="s">
+      <c r="M25" s="44" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3110,41 +3141,41 @@
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="53">
+      <c r="B27" s="52">
         <v>0.2</v>
       </c>
-      <c r="C27" s="52" t="s">
+      <c r="C27" s="51" t="s">
         <v>159</v>
       </c>
       <c r="H27" s="4"/>
-      <c r="I27" s="46" t="s">
+      <c r="I27" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="J27" s="47">
+      <c r="J27" s="46">
         <f>J26*B27</f>
         <v>7.9438666666666693</v>
       </c>
-      <c r="K27" s="48">
+      <c r="K27" s="47">
         <f>K26*B27</f>
         <v>4.6063733333333339</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="57"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="57"/>
+      <c r="A28" s="56"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="56"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="49" t="s">
+      <c r="I28" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="J28" s="50">
+      <c r="J28" s="49">
         <f>J26+J27</f>
         <v>47.663200000000018</v>
       </c>
-      <c r="K28" s="51">
+      <c r="K28" s="50">
         <f>K26+K27</f>
         <v>27.638240000000003</v>
       </c>
@@ -3368,7 +3399,7 @@
     <hyperlink ref="L12" r:id="rId15"/>
     <hyperlink ref="M12" r:id="rId16"/>
     <hyperlink ref="L13" r:id="rId17"/>
-    <hyperlink ref="M15" r:id="rId18"/>
+    <hyperlink ref="M14" r:id="rId18"/>
     <hyperlink ref="L16" r:id="rId19"/>
     <hyperlink ref="M16" r:id="rId20"/>
     <hyperlink ref="L17" r:id="rId21"/>
@@ -3384,8 +3415,8 @@
     <hyperlink ref="M23" r:id="rId31"/>
     <hyperlink ref="L25" r:id="rId32"/>
     <hyperlink ref="M25" r:id="rId33"/>
-    <hyperlink ref="L15" r:id="rId34"/>
-    <hyperlink ref="M14" r:id="rId35"/>
+    <hyperlink ref="L14" r:id="rId34"/>
+    <hyperlink ref="M15" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
@@ -3397,14 +3428,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="51.28515625" customWidth="1"/>
-    <col min="2" max="2" width="147.28515625" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
@@ -3415,10 +3448,51 @@
         <v>136</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>